<commit_message>
final self assessment data ethics
</commit_message>
<xml_diff>
--- a/final_documents/Self-Assessment_Data Ethics.xlsx
+++ b/final_documents/Self-Assessment_Data Ethics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\AI4Good\AI4Good\final_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64863F3D-A936-4D86-A93E-E8CC6CBEE510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44042EB3-DE23-4886-ACFB-019752E9C73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="12800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="179">
   <si>
     <t>Self-Assessment Form</t>
   </si>
@@ -614,6 +614,84 @@
   </si>
   <si>
     <t>Start date: 04.03.25 (Kick Off Climate), key dates: 24.03.25 (Meeting with Basil and project explanation), 25.03.25 (Milestone I), 15.04.25 (Milestone II), 12.05.25 (Milestone III), 24.05.25 (Final submission), end date: 26.05.25 (Presentation)</t>
+  </si>
+  <si>
+    <t>Interactive dashboard of runoff data and model sensitivity. Project partnes:  Gudmundsson Lukas and Kraft Basil, no sponsors.</t>
+  </si>
+  <si>
+    <t>How data are collected: Project data were provided by Kraft Basil. How was data used: Integration in interactive dashboard, ai training and calculation of model sensitivity. Research environment used: Python with VS Code and Pycharm.</t>
+  </si>
+  <si>
+    <t>https://www.research-collection.ethz.ch/handle/20.500.11850/714281, CH-RUN: Runoff reconstruction for Switzerland (CHRUN_v1)</t>
+  </si>
+  <si>
+    <t>No sensitive personal data.</t>
+  </si>
+  <si>
+    <t>Project includes linked data.</t>
+  </si>
+  <si>
+    <t>No patient level health data.</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Primary goal was visualisation of data and as supplement we implemented a sensitvity model.</t>
+  </si>
+  <si>
+    <t>Societal benefits might be limited to certain groups/areas</t>
+  </si>
+  <si>
+    <t>Groups that work with water runoff data in Switzerland.</t>
+  </si>
+  <si>
+    <t>No personal data used in the project. Probably wrong AI predictions could lead to wrong assumptions, if model predicts wrong sensitivity values.</t>
+  </si>
+  <si>
+    <t>The data was processed to the best of our knowledge and belief.</t>
+  </si>
+  <si>
+    <t>Data doesn't contains personal data.</t>
+  </si>
+  <si>
+    <t>Basic data security measures are in place (e.g. institutional storage ETH, version control), and no further special arrangements are currently required.</t>
+  </si>
+  <si>
+    <t>Data is based entirely on environmental and hydrological data (e.g., runoff, precipitation, temperature). Therefore, informed consent from data subjects was not required.</t>
+  </si>
+  <si>
+    <t>The dataset is publicly available.</t>
+  </si>
+  <si>
+    <t>A sensitivity-aware AI model was trained to assess differences between runoff models, increasing the robustness and reliability of the conclusions.</t>
+  </si>
+  <si>
+    <t>All research outputs, including automated model results, are subject to manual review to ensure accuracy and reliability throughout the project lifecycle.</t>
+  </si>
+  <si>
+    <t>The dataset is publicly available. Researchers involved in the project have received formal training in hydrological modeling and data management.</t>
+  </si>
+  <si>
+    <t>The project integrates SHAP (SHapley Additive exPlanations, gradient explainer) in Python to interpret the difference between the runoff models.</t>
+  </si>
+  <si>
+    <t>While the direct public benefit may not be immediate or easily quantifiable, the research advances understanding of model differences and uncertainty in runoff predictions.</t>
+  </si>
+  <si>
+    <t>Public views are at this moment unknown.</t>
+  </si>
+  <si>
+    <t>Public engagement was not part of the project goal.</t>
+  </si>
+  <si>
+    <t>Stored in gitlab repository.</t>
+  </si>
+  <si>
+    <t>The sharing of methods and tools has not yet been confirmed.</t>
+  </si>
+  <si>
+    <t>Public access to research outcomes is currently uncertain.</t>
   </si>
 </sst>
 </file>
@@ -1949,14 +2027,6 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="5" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -2388,6 +2458,337 @@
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -2432,351 +2833,28 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -3586,8 +3664,8 @@
   </sheetPr>
   <dimension ref="A1:XFC1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:L10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1048576" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N54" sqref="N54:O54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.35" zeroHeight="1" x14ac:dyDescent="0.5"/>
@@ -3631,12 +3709,12 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="42" t="s">
+      <c r="L1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
       <c r="P1" s="3"/>
     </row>
     <row r="2" spans="1:16 16381:16383" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
@@ -3677,32 +3755,32 @@
     </row>
     <row r="4" spans="1:16 16381:16383" s="4" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1"/>
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="177" t="s">
+      <c r="C4" s="204" t="s">
         <v>151</v>
       </c>
-      <c r="D4" s="178"/>
-      <c r="E4" s="178"/>
-      <c r="F4" s="178"/>
-      <c r="G4" s="178"/>
-      <c r="H4" s="178"/>
-      <c r="I4" s="178"/>
-      <c r="J4" s="178"/>
-      <c r="K4" s="178"/>
-      <c r="L4" s="179"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
+      <c r="D4" s="205"/>
+      <c r="E4" s="205"/>
+      <c r="F4" s="205"/>
+      <c r="G4" s="205"/>
+      <c r="H4" s="205"/>
+      <c r="I4" s="205"/>
+      <c r="J4" s="205"/>
+      <c r="K4" s="205"/>
+      <c r="L4" s="206"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
       <c r="P4" s="11"/>
-      <c r="XFA4" s="76" t="s">
+      <c r="XFA4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="XFB4" s="76" t="s">
+      <c r="XFB4" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="XFC4" s="76" t="s">
+      <c r="XFC4" s="74" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3718,161 +3796,161 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="9"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
       <c r="P5" s="11"/>
-      <c r="XFA5" s="77"/>
-      <c r="XFB5" s="77"/>
-      <c r="XFC5" s="77"/>
+      <c r="XFA5" s="75"/>
+      <c r="XFB5" s="75"/>
+      <c r="XFC5" s="75"/>
     </row>
     <row r="6" spans="1:16 16381:16383" s="4" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1"/>
-      <c r="B6" s="190" t="s">
+      <c r="B6" s="217" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="186" t="s">
+      <c r="C6" s="213" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="186"/>
-      <c r="E6" s="186"/>
-      <c r="F6" s="186"/>
-      <c r="G6" s="186"/>
-      <c r="H6" s="186"/>
-      <c r="I6" s="186"/>
-      <c r="J6" s="186"/>
-      <c r="K6" s="186"/>
-      <c r="L6" s="186"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
+      <c r="D6" s="213"/>
+      <c r="E6" s="213"/>
+      <c r="F6" s="213"/>
+      <c r="G6" s="213"/>
+      <c r="H6" s="213"/>
+      <c r="I6" s="213"/>
+      <c r="J6" s="213"/>
+      <c r="K6" s="213"/>
+      <c r="L6" s="213"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
       <c r="P6" s="11"/>
-      <c r="XFA6" s="78" t="s">
+      <c r="XFA6" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="XFB6" s="78" t="s">
+      <c r="XFB6" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="XFC6" s="78" t="s">
+      <c r="XFC6" s="76" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:16 16381:16383" s="4" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1"/>
-      <c r="B7" s="190"/>
-      <c r="C7" s="177" t="s">
+      <c r="B7" s="217"/>
+      <c r="C7" s="204" t="s">
         <v>152</v>
       </c>
-      <c r="D7" s="178"/>
-      <c r="E7" s="178"/>
-      <c r="F7" s="178"/>
-      <c r="G7" s="178"/>
-      <c r="H7" s="178"/>
-      <c r="I7" s="178"/>
-      <c r="J7" s="178"/>
-      <c r="K7" s="178"/>
-      <c r="L7" s="179"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="47"/>
+      <c r="D7" s="205"/>
+      <c r="E7" s="205"/>
+      <c r="F7" s="205"/>
+      <c r="G7" s="205"/>
+      <c r="H7" s="205"/>
+      <c r="I7" s="205"/>
+      <c r="J7" s="205"/>
+      <c r="K7" s="205"/>
+      <c r="L7" s="206"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="45"/>
       <c r="P7" s="11"/>
-      <c r="XFA7" s="78" t="s">
+      <c r="XFA7" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="XFB7" s="84" t="s">
+      <c r="XFB7" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="XFC7" s="78" t="s">
+      <c r="XFC7" s="76" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:16 16381:16383" s="4" customFormat="1" ht="8.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="192"/>
-      <c r="D8" s="192"/>
-      <c r="E8" s="192"/>
-      <c r="F8" s="192"/>
-      <c r="G8" s="192"/>
-      <c r="H8" s="192"/>
-      <c r="I8" s="192"/>
-      <c r="J8" s="192"/>
-      <c r="K8" s="192"/>
-      <c r="L8" s="192"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
+      <c r="C8" s="219"/>
+      <c r="D8" s="219"/>
+      <c r="E8" s="219"/>
+      <c r="F8" s="219"/>
+      <c r="G8" s="219"/>
+      <c r="H8" s="219"/>
+      <c r="I8" s="219"/>
+      <c r="J8" s="219"/>
+      <c r="K8" s="219"/>
+      <c r="L8" s="219"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="45"/>
       <c r="P8" s="11"/>
-      <c r="XFA8" s="133" t="s">
+      <c r="XFA8" s="131" t="s">
         <v>14</v>
       </c>
-      <c r="XFB8" s="85" t="s">
+      <c r="XFB8" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="XFC8" s="79" t="s">
+      <c r="XFC8" s="77" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:16 16381:16383" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1"/>
-      <c r="B9" s="191" t="s">
+      <c r="B9" s="218" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="187" t="s">
+      <c r="C9" s="214" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="187"/>
-      <c r="E9" s="187"/>
-      <c r="F9" s="187"/>
-      <c r="G9" s="187"/>
-      <c r="H9" s="187"/>
-      <c r="I9" s="187"/>
-      <c r="J9" s="187"/>
-      <c r="K9" s="187"/>
-      <c r="L9" s="187"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="47"/>
+      <c r="D9" s="214"/>
+      <c r="E9" s="214"/>
+      <c r="F9" s="214"/>
+      <c r="G9" s="214"/>
+      <c r="H9" s="214"/>
+      <c r="I9" s="214"/>
+      <c r="J9" s="214"/>
+      <c r="K9" s="214"/>
+      <c r="L9" s="214"/>
+      <c r="M9" s="45"/>
+      <c r="N9" s="45"/>
+      <c r="O9" s="45"/>
       <c r="P9" s="11"/>
-      <c r="XFA9" s="76" t="s">
+      <c r="XFA9" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="XFB9" s="76" t="s">
+      <c r="XFB9" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="XFC9" s="76" t="s">
+      <c r="XFC9" s="74" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:16 16381:16383" s="4" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="1"/>
-      <c r="B10" s="191"/>
-      <c r="C10" s="177">
-        <v>0</v>
-      </c>
-      <c r="D10" s="178"/>
-      <c r="E10" s="178"/>
-      <c r="F10" s="178"/>
-      <c r="G10" s="178"/>
-      <c r="H10" s="178"/>
-      <c r="I10" s="178"/>
-      <c r="J10" s="178"/>
-      <c r="K10" s="178"/>
-      <c r="L10" s="179"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="132" t="s">
+      <c r="B10" s="218"/>
+      <c r="C10" s="204" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="205"/>
+      <c r="E10" s="205"/>
+      <c r="F10" s="205"/>
+      <c r="G10" s="205"/>
+      <c r="H10" s="205"/>
+      <c r="I10" s="205"/>
+      <c r="J10" s="205"/>
+      <c r="K10" s="205"/>
+      <c r="L10" s="206"/>
+      <c r="M10" s="45"/>
+      <c r="N10" s="130" t="s">
         <v>22</v>
       </c>
-      <c r="O10" s="47"/>
+      <c r="O10" s="45"/>
       <c r="P10" s="11"/>
-      <c r="XFA10" s="78" t="s">
+      <c r="XFA10" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="XFB10" s="84" t="s">
+      <c r="XFB10" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="XFC10" s="78" t="s">
+      <c r="XFC10" s="76" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3892,70 +3970,72 @@
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="11"/>
-      <c r="XFA11" s="81" t="s">
+      <c r="XFA11" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="XFB11" s="78" t="s">
+      <c r="XFB11" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="XFC11" s="78" t="s">
+      <c r="XFC11" s="76" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:16 16381:16383" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1"/>
-      <c r="B12" s="191" t="s">
+      <c r="B12" s="218" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="188" t="s">
+      <c r="C12" s="215" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="188"/>
-      <c r="E12" s="188"/>
-      <c r="F12" s="188"/>
-      <c r="G12" s="188"/>
-      <c r="H12" s="188"/>
-      <c r="I12" s="188"/>
-      <c r="J12" s="188"/>
-      <c r="K12" s="188"/>
-      <c r="L12" s="188"/>
+      <c r="D12" s="215"/>
+      <c r="E12" s="215"/>
+      <c r="F12" s="215"/>
+      <c r="G12" s="215"/>
+      <c r="H12" s="215"/>
+      <c r="I12" s="215"/>
+      <c r="J12" s="215"/>
+      <c r="K12" s="215"/>
+      <c r="L12" s="215"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
       <c r="P12" s="11"/>
-      <c r="XFA12" s="81" t="s">
+      <c r="XFA12" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="XFB12" s="85" t="s">
+      <c r="XFB12" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="XFC12" s="78" t="s">
+      <c r="XFC12" s="76" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:16 16381:16383" s="4" customFormat="1" ht="205.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="1"/>
-      <c r="B13" s="191"/>
-      <c r="C13" s="180"/>
-      <c r="D13" s="181"/>
-      <c r="E13" s="181"/>
-      <c r="F13" s="181"/>
-      <c r="G13" s="181"/>
-      <c r="H13" s="181"/>
-      <c r="I13" s="181"/>
-      <c r="J13" s="181"/>
-      <c r="K13" s="181"/>
-      <c r="L13" s="182"/>
-      <c r="N13" s="67"/>
-      <c r="O13" s="67"/>
+      <c r="B13" s="218"/>
+      <c r="C13" s="207" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="208"/>
+      <c r="E13" s="208"/>
+      <c r="F13" s="208"/>
+      <c r="G13" s="208"/>
+      <c r="H13" s="208"/>
+      <c r="I13" s="208"/>
+      <c r="J13" s="208"/>
+      <c r="K13" s="208"/>
+      <c r="L13" s="209"/>
+      <c r="N13" s="65"/>
+      <c r="O13" s="65"/>
       <c r="P13" s="11"/>
-      <c r="XFA13" s="82" t="s">
+      <c r="XFA13" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="XFB13" s="76" t="s">
+      <c r="XFB13" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="XFC13" s="79" t="s">
+      <c r="XFC13" s="77" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3971,76 +4051,78 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="12"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="40"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
       <c r="P14" s="11"/>
-      <c r="XFA14" s="76" t="s">
+      <c r="XFA14" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="XFB14" s="84" t="s">
+      <c r="XFB14" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="XFC14" s="76" t="s">
+      <c r="XFC14" s="74" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:16 16381:16383" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1"/>
-      <c r="B15" s="191" t="s">
+      <c r="B15" s="218" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="189" t="s">
+      <c r="C15" s="216" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="189"/>
-      <c r="E15" s="189"/>
-      <c r="F15" s="189"/>
-      <c r="G15" s="189"/>
-      <c r="H15" s="189"/>
-      <c r="I15" s="189"/>
-      <c r="J15" s="189"/>
-      <c r="K15" s="189"/>
-      <c r="L15" s="189"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="40"/>
-      <c r="O15" s="40"/>
+      <c r="D15" s="216"/>
+      <c r="E15" s="216"/>
+      <c r="F15" s="216"/>
+      <c r="G15" s="216"/>
+      <c r="H15" s="216"/>
+      <c r="I15" s="216"/>
+      <c r="J15" s="216"/>
+      <c r="K15" s="216"/>
+      <c r="L15" s="216"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
       <c r="P15" s="11"/>
-      <c r="XFA15" s="81" t="s">
+      <c r="XFA15" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="XFB15" s="84" t="s">
+      <c r="XFB15" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="XFC15" s="78" t="s">
+      <c r="XFC15" s="76" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:16 16381:16383" s="4" customFormat="1" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1"/>
-      <c r="B16" s="191"/>
-      <c r="C16" s="183"/>
-      <c r="D16" s="184"/>
-      <c r="E16" s="184"/>
-      <c r="F16" s="184"/>
-      <c r="G16" s="184"/>
-      <c r="H16" s="184"/>
-      <c r="I16" s="184"/>
-      <c r="J16" s="184"/>
-      <c r="K16" s="184"/>
-      <c r="L16" s="185"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="41"/>
+      <c r="B16" s="218"/>
+      <c r="C16" s="210" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" s="211"/>
+      <c r="E16" s="211"/>
+      <c r="F16" s="211"/>
+      <c r="G16" s="211"/>
+      <c r="H16" s="211"/>
+      <c r="I16" s="211"/>
+      <c r="J16" s="211"/>
+      <c r="K16" s="211"/>
+      <c r="L16" s="212"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
       <c r="P16" s="11"/>
-      <c r="XFA16" s="78" t="s">
+      <c r="XFA16" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="XFB16" s="85" t="s">
+      <c r="XFB16" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="XFC16" s="78" t="s">
+      <c r="XFC16" s="76" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4061,21 +4143,21 @@
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
       <c r="P17" s="11"/>
-      <c r="XFA17" s="82" t="s">
+      <c r="XFA17" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="XFB17" s="76" t="s">
+      <c r="XFB17" s="74" t="s">
         <v>49</v>
       </c>
-      <c r="XFC17" s="79" t="s">
+      <c r="XFC17" s="77" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:18 16381:16383" s="4" customFormat="1" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
@@ -4088,258 +4170,266 @@
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" s="11"/>
-      <c r="XFA18" s="76" t="s">
+      <c r="XFA18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="XFB18" s="78" t="s">
+      <c r="XFB18" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="XFC18" s="92" t="s">
+      <c r="XFC18" s="90" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:18 16381:16383" s="4" customFormat="1" ht="58.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1"/>
-      <c r="B19" s="170" t="str">
+      <c r="B19" s="197" t="str">
         <f>IF(SUM(I20:I24)=0,"Have you considered these questions?","")</f>
-        <v>Have you considered these questions?</v>
-      </c>
-      <c r="C19" s="171"/>
+        <v/>
+      </c>
+      <c r="C19" s="198"/>
       <c r="D19" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="77"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="70" t="s">
+      <c r="E19" s="75"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="I19" s="68" t="s">
+      <c r="I19" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="J19" s="66"/>
-      <c r="K19" s="71"/>
-      <c r="L19" s="223" t="s">
+      <c r="J19" s="64"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="144" t="s">
         <v>57</v>
       </c>
-      <c r="M19" s="224"/>
-      <c r="N19" s="225"/>
-      <c r="O19" s="62"/>
+      <c r="M19" s="145"/>
+      <c r="N19" s="146"/>
+      <c r="O19" s="60"/>
       <c r="P19" s="11"/>
-      <c r="XFA19" s="78" t="s">
+      <c r="XFA19" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="XFB19" s="78" t="s">
+      <c r="XFB19" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="XFC19" s="78" t="s">
+      <c r="XFC19" s="76" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:18 16381:16383" s="4" customFormat="1" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1"/>
-      <c r="B20" s="162" t="s">
+      <c r="B20" s="189" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="163"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="136" t="s">
+      <c r="C20" s="190"/>
+      <c r="D20" s="235" t="s">
+        <v>157</v>
+      </c>
+      <c r="E20" s="134" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="65"/>
-      <c r="H20" s="59">
+      <c r="G20" s="63"/>
+      <c r="H20" s="57">
         <f>IF(D20=1, 1+0.05, 1)</f>
         <v>1</v>
       </c>
-      <c r="I20" s="66">
+      <c r="I20" s="64">
         <f>IF(ISBLANK(D20),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="J20" s="66"/>
-      <c r="K20" s="71"/>
-      <c r="L20" s="226"/>
-      <c r="M20" s="227"/>
-      <c r="N20" s="228"/>
-      <c r="O20" s="62"/>
-      <c r="R20" s="134" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" s="64"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="147"/>
+      <c r="M20" s="148"/>
+      <c r="N20" s="149"/>
+      <c r="O20" s="60"/>
+      <c r="R20" s="132" t="s">
         <v>63</v>
       </c>
-      <c r="XFA20" s="78" t="s">
+      <c r="XFA20" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="XFB20" s="78" t="s">
+      <c r="XFB20" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="XFC20" s="78" t="s">
+      <c r="XFC20" s="76" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:18 16381:16383" s="4" customFormat="1" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1"/>
-      <c r="B21" s="164" t="s">
+      <c r="B21" s="191" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="165"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="115">
+      <c r="C21" s="192"/>
+      <c r="D21" s="236" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="113">
         <f>IF(COUNTBLANK($N$28:$N$55)&gt;0,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="G21" s="65"/>
-      <c r="H21" s="59">
+        <v>0</v>
+      </c>
+      <c r="G21" s="63"/>
+      <c r="H21" s="57">
         <f>IF(D21=1, 1+0.1, 1)</f>
         <v>1</v>
       </c>
-      <c r="I21" s="66">
+      <c r="I21" s="64">
         <f>IF(ISBLANK(D21),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="J21" s="72"/>
-      <c r="K21" s="71"/>
-      <c r="L21" s="174" t="str">
+        <v>1</v>
+      </c>
+      <c r="J21" s="70"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="201" t="str">
         <f>IF(AND($E$21=1,$E$24&gt;=1),"-",IF($E$24&gt;=1,"-",IF($E$21=1,"-",IF($R$21&lt;1,"Green",IF(AND($R$21&gt;=1,$R$21&lt;1.6),"Green",IF(AND($R$21&gt;=1.6,$R$21&lt;2.3),"Amber",IF(AND($R$21&gt;=2.3,$R$21&lt;3),"Red",IF(AND($R$21&gt;=3,$R$21&lt;=100),"Red","-"))))))))</f>
-        <v>-</v>
-      </c>
-      <c r="M21" s="217" t="str">
+        <v>Amber</v>
+      </c>
+      <c r="M21" s="138" t="str">
         <f>IF(AND($E$21=1,$E$24&gt;=1),"Form not complete, please select an option in each of the drop down boxes and provide justifications",IF($E$24&gt;=1,"Form not complete, please select an option in each of the drop down boxes",IF($E$21=1,"One or more justifications have been left blank, please complete all justifications as per the justification suggestion",IF(SUM(P27:P55)&gt;0,"One or more items have reached or exceeded a tolerance level - consult with the Data Ethics team",IF($R$21&lt;1,"Very low risk - project may proceed after confirmation from the Data Ethics team",IF(AND($R$21&gt;=1,$R$21&lt;1.6),"Low risk - project may proceed after confirmation from the Data Ethics team",IF(AND($R$21&gt;=1.6,$R$21&lt;2.3),"Average risk - consult with the Data Ethics team to discuss actions to mitigate any highlighted risks before proceeding with the project",IF(AND($R$21&gt;=2.3,$R$21&lt;3),"High risk - consult with the Data Ethics team. If risks cannot be mitigated then this project should be presented to NSDEC for a full independent ethical review before proceeding",IF(AND($R$21&gt;=3,$R$21&lt;=100),"Very High risk - consult with the Data Ethics team. If risks cannot be mitigated then this project should be presented to NSDEC for a full independent ethical review before proceeding","Project requires an ethical review before proceeding, please select an option in each of the drop down boxes")))))))))</f>
-        <v>Form not complete, please select an option in each of the drop down boxes and provide justifications</v>
-      </c>
-      <c r="N21" s="218"/>
-      <c r="O21" s="128"/>
-      <c r="R21" s="135" t="str">
+        <v>One or more items have reached or exceeded a tolerance level - consult with the Data Ethics team</v>
+      </c>
+      <c r="N21" s="139"/>
+      <c r="O21" s="126"/>
+      <c r="R21" s="133">
         <f>IFERROR(AVERAGE(K30,K36,K42,K47,K50,K53)*PRODUCT($H$20:$H$23),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="XFA21" s="79" t="s">
+        <v>1.622222222222222</v>
+      </c>
+      <c r="XFA21" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="XFB21" s="79" t="s">
+      <c r="XFB21" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="XFC21" s="78" t="s">
+      <c r="XFC21" s="76" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:18 16381:16383" s="4" customFormat="1" ht="48.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1"/>
-      <c r="B22" s="166" t="s">
+      <c r="B22" s="193" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="167"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="115">
+      <c r="C22" s="194"/>
+      <c r="D22" s="236" t="s">
+        <v>158</v>
+      </c>
+      <c r="E22" s="113">
         <f>IF(COUNTBLANK($D$30:$D$55)&gt;0,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="G22" s="65"/>
-      <c r="H22" s="59">
+        <v>0</v>
+      </c>
+      <c r="G22" s="63"/>
+      <c r="H22" s="57">
         <f>IF(D22=1, 1+0.2, 1)</f>
         <v>1</v>
       </c>
-      <c r="I22" s="66">
+      <c r="I22" s="64">
         <f>IF(ISBLANK(D22),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="J22" s="66"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="175"/>
-      <c r="M22" s="219"/>
-      <c r="N22" s="220"/>
-      <c r="O22" s="63"/>
-      <c r="XFA22" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" s="64"/>
+      <c r="K22" s="69"/>
+      <c r="L22" s="202"/>
+      <c r="M22" s="140"/>
+      <c r="N22" s="141"/>
+      <c r="O22" s="61"/>
+      <c r="XFA22" s="74" t="s">
         <v>72</v>
       </c>
-      <c r="XFB22" s="76" t="s">
+      <c r="XFB22" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="XFC22" s="79" t="s">
+      <c r="XFC22" s="77" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:18 16381:16383" s="4" customFormat="1" ht="101.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1"/>
-      <c r="B23" s="168" t="s">
+      <c r="B23" s="195" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="169"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="115">
+      <c r="C23" s="196"/>
+      <c r="D23" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="E23" s="113">
         <f>IF(COUNTBLANK($E$29)&gt;0,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="G23" s="65"/>
-      <c r="H23" s="59">
+        <v>0</v>
+      </c>
+      <c r="G23" s="63"/>
+      <c r="H23" s="57">
         <f>IF(D23=1, 1+0.2, 1)</f>
         <v>1</v>
       </c>
-      <c r="I23" s="66">
+      <c r="I23" s="64">
         <f>IF(ISBLANK(D23),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="J23" s="66"/>
-      <c r="K23" s="71"/>
-      <c r="L23" s="175"/>
-      <c r="M23" s="219"/>
-      <c r="N23" s="220"/>
-      <c r="O23" s="63"/>
-      <c r="XFA23" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="64"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="202"/>
+      <c r="M23" s="140"/>
+      <c r="N23" s="141"/>
+      <c r="O23" s="61"/>
+      <c r="XFA23" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="XFB23" s="78" t="s">
+      <c r="XFB23" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="XFC23" s="92" t="s">
+      <c r="XFC23" s="90" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:18 16381:16383" s="4" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1"/>
-      <c r="B24" s="140"/>
-      <c r="C24" s="141"/>
-      <c r="D24" s="119"/>
-      <c r="E24" s="137">
+      <c r="B24" s="221"/>
+      <c r="C24" s="222"/>
+      <c r="D24" s="117"/>
+      <c r="E24" s="135">
         <f>SUM($E$22,$E$23)</f>
-        <v>2</v>
-      </c>
-      <c r="G24" s="65"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="71"/>
-      <c r="L24" s="176"/>
-      <c r="M24" s="221"/>
-      <c r="N24" s="222"/>
-      <c r="O24" s="63"/>
-      <c r="XFA24" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" s="63"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="203"/>
+      <c r="M24" s="142"/>
+      <c r="N24" s="143"/>
+      <c r="O24" s="61"/>
+      <c r="XFA24" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="XFB24" s="78" t="s">
+      <c r="XFB24" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="XFC24" s="78" t="s">
+      <c r="XFC24" s="76" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:18 16381:16383" s="4" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="138"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="75"/>
-      <c r="K25" s="75"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="136"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73"/>
       <c r="L25" s="14"/>
       <c r="M25" s="14"/>
-      <c r="XFA25" s="79" t="s">
+      <c r="XFA25" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="XFB25" s="78" t="s">
+      <c r="XFB25" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="XFC25" s="78" t="s">
+      <c r="XFC25" s="76" t="s">
         <v>84</v>
       </c>
     </row>
@@ -4357,70 +4447,70 @@
       <c r="K26" s="9"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
-      <c r="N26" s="48"/>
-      <c r="O26" s="48"/>
+      <c r="N26" s="46"/>
+      <c r="O26" s="46"/>
       <c r="P26" s="11"/>
-      <c r="XFA26" s="92" t="s">
+      <c r="XFA26" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="XFB26" s="79" t="s">
+      <c r="XFB26" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="XFC26" s="78" t="s">
+      <c r="XFC26" s="76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:18 16381:16383" ht="127.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="58"/>
-      <c r="C27" s="57" t="s">
+      <c r="B27" s="56"/>
+      <c r="C27" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="172" t="s">
+      <c r="D27" s="199" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="173"/>
+      <c r="E27" s="200"/>
       <c r="F27" s="15"/>
-      <c r="G27" s="154" t="s">
+      <c r="G27" s="231" t="s">
         <v>90</v>
       </c>
-      <c r="H27" s="155"/>
-      <c r="I27" s="155"/>
-      <c r="J27" s="156"/>
-      <c r="K27" s="49" t="s">
+      <c r="H27" s="232"/>
+      <c r="I27" s="232"/>
+      <c r="J27" s="233"/>
+      <c r="K27" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="L27" s="198" t="s">
+      <c r="L27" s="181" t="s">
         <v>92</v>
       </c>
-      <c r="M27" s="199"/>
-      <c r="N27" s="208" t="s">
+      <c r="M27" s="182"/>
+      <c r="N27" s="166" t="s">
         <v>93</v>
       </c>
-      <c r="O27" s="209"/>
+      <c r="O27" s="167"/>
       <c r="P27" s="16"/>
-      <c r="XFA27" s="83" t="s">
+      <c r="XFA27" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="XFB27" s="88" t="s">
+      <c r="XFB27" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="XFC27" s="87" t="s">
+      <c r="XFC27" s="85" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:18 16381:16383" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="80"/>
-      <c r="B28" s="114" t="s">
+      <c r="A28" s="78"/>
+      <c r="B28" s="112" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="56" t="s">
+      <c r="C28" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="193" t="s">
+      <c r="D28" s="176" t="s">
         <v>99</v>
       </c>
-      <c r="E28" s="160"/>
-      <c r="F28" s="37" t="s">
+      <c r="E28" s="175"/>
+      <c r="F28" s="35" t="s">
         <v>100</v>
       </c>
       <c r="G28" s="18">
@@ -4432,242 +4522,258 @@
       <c r="I28" s="19">
         <v>3</v>
       </c>
-      <c r="J28" s="25" t="s">
+      <c r="J28" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="K28" s="69" t="str">
+      <c r="K28" s="67">
         <f>K31</f>
-        <v>-</v>
-      </c>
-      <c r="L28" s="152" t="s">
+        <v>1.5</v>
+      </c>
+      <c r="L28" s="150" t="s">
         <v>102</v>
       </c>
-      <c r="M28" s="153"/>
-      <c r="N28" s="152" t="s">
+      <c r="M28" s="151"/>
+      <c r="N28" s="150" t="s">
         <v>103</v>
       </c>
-      <c r="O28" s="153"/>
-      <c r="XFA28" s="84" t="s">
+      <c r="O28" s="151"/>
+      <c r="XFA28" s="82" t="s">
         <v>104</v>
       </c>
-      <c r="XFB28" s="83" t="s">
+      <c r="XFB28" s="81" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:18 16381:16383" s="50" customFormat="1" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:18 16381:16383" s="48" customFormat="1" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1"/>
-      <c r="B29" s="51">
+      <c r="B29" s="49">
         <v>1</v>
       </c>
-      <c r="C29" s="130" t="s">
+      <c r="C29" s="128" t="s">
         <v>106</v>
       </c>
-      <c r="D29" s="131" t="s">
+      <c r="D29" s="129" t="s">
         <v>107</v>
       </c>
-      <c r="E29" s="129"/>
-      <c r="F29" s="35" t="str">
+      <c r="E29" s="127" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="33">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G29:$I29,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G29" s="97" t="str">
+        <v>2</v>
+      </c>
+      <c r="G29" s="95" t="str">
         <f>IF($E$29="This research will provide a significant public good in line with best practice guidance",1,"")</f>
         <v/>
       </c>
-      <c r="H29" s="98" t="str">
+      <c r="H29" s="96">
         <f>IF($E$29="Potential to achieve Public Good which requires further exploration",1,"")</f>
-        <v/>
-      </c>
-      <c r="I29" s="98" t="str">
+        <v>1</v>
+      </c>
+      <c r="I29" s="96" t="str">
         <f>IF($E$29="Negligible public good that is not in line with best practice guidance",1,"")</f>
         <v/>
       </c>
-      <c r="J29" s="26"/>
-      <c r="K29" s="32" t="str">
+      <c r="J29" s="24"/>
+      <c r="K29" s="30">
         <f>K30</f>
-        <v>-</v>
-      </c>
-      <c r="L29" s="206" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="L29" s="164" t="str">
         <f>IF($F$29=1,"Please explain the public good for this project. A link to our public good guidance can be found to the left of the drop down statement",IF($F$29=2,"This selection has passed a tolerance. Please explain the potential public good, and what is to be done to further explore this potential",IF($F$29=3,"This selection has passed a tolerance. Please explain why there is not a public good","Please select an option in cell D29")))</f>
-        <v>Please select an option in cell D29</v>
-      </c>
-      <c r="M29" s="207"/>
-      <c r="N29" s="210"/>
-      <c r="O29" s="211"/>
+        <v>This selection has passed a tolerance. Please explain the potential public good, and what is to be done to further explore this potential</v>
+      </c>
+      <c r="M29" s="165"/>
+      <c r="N29" s="152" t="s">
+        <v>160</v>
+      </c>
+      <c r="O29" s="153"/>
       <c r="P29" s="16">
         <f>IF(SUM(H29:I29)&gt;0, 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="XFA29" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="XFA29" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="XFB29" s="93" t="s">
+      <c r="XFB29" s="91" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:18 16381:16383" s="50" customFormat="1" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:18 16381:16383" s="48" customFormat="1" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1"/>
-      <c r="B30" s="52">
+      <c r="B30" s="50">
         <f>IF(IFERROR(SEARCH("Principle", C30, 1)&gt; 1, -1)=-1, B29+1, B29)</f>
         <v>2</v>
       </c>
-      <c r="C30" s="120" t="s">
+      <c r="C30" s="118" t="s">
         <v>110</v>
       </c>
-      <c r="D30" s="194"/>
-      <c r="E30" s="195"/>
-      <c r="F30" s="35" t="str">
+      <c r="D30" s="177" t="s">
+        <v>161</v>
+      </c>
+      <c r="E30" s="178"/>
+      <c r="F30" s="33">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G30:$I30,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G30" s="99" t="str">
+        <v>2</v>
+      </c>
+      <c r="G30" s="97" t="str">
         <f>IF($D$30="Public good applicable to entire population",1,"")</f>
         <v/>
       </c>
-      <c r="H30" s="100" t="str">
+      <c r="H30" s="98">
         <f>IF($D$30="Societal benefits might be limited to certain groups/areas",1,"")</f>
-        <v/>
-      </c>
-      <c r="I30" s="101" t="str">
+        <v>1</v>
+      </c>
+      <c r="I30" s="99" t="str">
         <f>IF($D$30="Societal benefits will be limited to certain groups/areas",1,"")</f>
         <v/>
       </c>
-      <c r="J30" s="102" t="str">
+      <c r="J30" s="100" t="str">
         <f>IF($D$30="N/A: Omit this item when the scope of this research specifically targets a particular group",1,"")</f>
         <v/>
       </c>
-      <c r="K30" s="32" t="str">
+      <c r="K30" s="30">
         <f>IFERROR(AVERAGE(F29:F32),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="L30" s="206" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="L30" s="164" t="str">
         <f>IF($F$30=1,"Please explain how the public good is applicable to the whole population",IF($F$30=2,"Please explain why this is proportional, and provide any mitigations against this limitation",IF($F$30=3,"This selection has passed a tolerance. Please explain why this is limited to certain groups, and provide any mitigations",IF($J$30=1,"Please explain why the research is focused on that specific group, and whether this, or other groups, might be adversely affected by this research","Please select an option in cell D30"))))</f>
-        <v>Please select an option in cell D30</v>
-      </c>
-      <c r="M30" s="207"/>
-      <c r="N30" s="212"/>
-      <c r="O30" s="213"/>
+        <v>Please explain why this is proportional, and provide any mitigations against this limitation</v>
+      </c>
+      <c r="M30" s="165"/>
+      <c r="N30" s="158" t="s">
+        <v>162</v>
+      </c>
+      <c r="O30" s="159"/>
       <c r="P30" s="16">
         <f>IF(SUM(I30:I30)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="XFA30" s="86" t="s">
+      <c r="XFA30" s="84" t="s">
         <v>111</v>
       </c>
-      <c r="XFB30" s="94" t="s">
+      <c r="XFB30" s="92" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:18 16381:16383" s="50" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:18 16381:16383" s="48" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A31" s="1"/>
-      <c r="B31" s="52">
+      <c r="B31" s="50">
         <f t="shared" ref="B31:B55" si="0">IF(IFERROR(SEARCH("Principle", C31, 1)&gt; 1, -1)=-1, B30+1, B30)</f>
         <v>3</v>
       </c>
-      <c r="C31" s="120" t="s">
+      <c r="C31" s="118" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="150"/>
-      <c r="E31" s="151"/>
-      <c r="F31" s="35" t="str">
+      <c r="D31" s="170" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="171"/>
+      <c r="F31" s="33">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G31:$I31,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G31" s="97" t="str">
+        <v>1</v>
+      </c>
+      <c r="G31" s="95">
         <f>IF($D$31="Negligible harm to anyone involved, including the public",1,"")</f>
-        <v/>
-      </c>
-      <c r="H31" s="113" t="str">
+        <v>1</v>
+      </c>
+      <c r="H31" s="111" t="str">
         <f>IF($D$31="Identified potential harm to anyone involved that can be justified and mitigated against",1,"")</f>
         <v/>
       </c>
-      <c r="I31" s="98" t="str">
+      <c r="I31" s="96" t="str">
         <f>IF($D$31="Identified potential harm that cannot be mitigated against",1,"")</f>
         <v/>
       </c>
-      <c r="J31" s="27"/>
-      <c r="K31" s="46" t="str">
+      <c r="J31" s="25"/>
+      <c r="K31" s="44">
         <f>K30</f>
-        <v>-</v>
-      </c>
-      <c r="L31" s="206" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="L31" s="164" t="str">
         <f>IF($F$31=1,"Please explain steps to ensure that there is no potential harm. This includes any potential harm as a result of secondary analysis outcomes",IF($F$31=2,"Please explain why this is proportional, and provide any mitigations against this potential harm",IF($F$31=3,"This selection has passed a tolerance. Please explain this potential harm and why it cannot be mitigated","Please select an option in cell D31")))</f>
-        <v>Please select an option in cell D31</v>
-      </c>
-      <c r="M31" s="207"/>
-      <c r="N31" s="214"/>
-      <c r="O31" s="215"/>
+        <v>Please explain steps to ensure that there is no potential harm. This includes any potential harm as a result of secondary analysis outcomes</v>
+      </c>
+      <c r="M31" s="165"/>
+      <c r="N31" s="168" t="s">
+        <v>163</v>
+      </c>
+      <c r="O31" s="169"/>
       <c r="P31" s="16">
         <f>IF(SUM(I31)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="XFA31" s="93" t="s">
+      <c r="XFA31" s="91" t="s">
         <v>114</v>
       </c>
-      <c r="XFB31" s="89" t="s">
+      <c r="XFB31" s="87" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="32" spans="1:18 16381:16383" s="50" customFormat="1" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:18 16381:16383" s="48" customFormat="1" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1"/>
-      <c r="B32" s="53">
+      <c r="B32" s="51">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C32" s="121" t="s">
+      <c r="C32" s="119" t="s">
         <v>116</v>
       </c>
-      <c r="D32" s="196"/>
-      <c r="E32" s="197"/>
-      <c r="F32" s="36" t="str">
+      <c r="D32" s="179" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="180"/>
+      <c r="F32" s="34">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G32:$I32,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G32" s="99" t="str">
+        <v>1</v>
+      </c>
+      <c r="G32" s="97">
         <f>IF($D$32="As yet, bias has not been identified in planned methods and outcomes",1,"")</f>
-        <v/>
-      </c>
-      <c r="H32" s="100" t="str">
+        <v>1</v>
+      </c>
+      <c r="H32" s="98" t="str">
         <f>IF($D$32="As yet, there is potential for bias/bias has been identified, but it can be justified and mitigated against",1,"")</f>
         <v/>
       </c>
-      <c r="I32" s="101" t="str">
+      <c r="I32" s="99" t="str">
         <f>IF($D$32="As yet, there is potential for bias/bias has been identified, but it cannot be mitigated against",1,"")</f>
         <v/>
       </c>
-      <c r="J32" s="28"/>
-      <c r="K32" s="33" t="str">
+      <c r="J32" s="26"/>
+      <c r="K32" s="31">
         <f>K30</f>
-        <v>-</v>
-      </c>
-      <c r="L32" s="206" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="L32" s="164" t="str">
         <f>IF($F$32=1,"Please explain steps taken to ensure that there is no bias",IF($F$32=2,"Please explain why this is proportional, and provide any mitigations against this bias",IF($F$32=3,"This selection has passed a tolerance. Please explain this bias and why it cannot be mitigated","Please select an option in cell D32")))</f>
-        <v>Please select an option in cell D32</v>
-      </c>
-      <c r="M32" s="207"/>
-      <c r="N32" s="235"/>
-      <c r="O32" s="236"/>
+        <v>Please explain steps taken to ensure that there is no bias</v>
+      </c>
+      <c r="M32" s="165"/>
+      <c r="N32" s="162" t="s">
+        <v>164</v>
+      </c>
+      <c r="O32" s="163"/>
       <c r="P32" s="16">
         <f>IF(SUM(I32)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="XFA32" s="93" t="s">
+      <c r="XFA32" s="91" t="s">
         <v>117</v>
       </c>
-      <c r="XFB32" s="90" t="s">
+      <c r="XFB32" s="88" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="33" spans="2:16 16381:16383" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="20"/>
-      <c r="C33" s="56" t="s">
+      <c r="C33" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="D33" s="159" t="s">
+      <c r="D33" s="234" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="160"/>
-      <c r="F33" s="37" t="s">
+      <c r="E33" s="175"/>
+      <c r="F33" s="35" t="s">
         <v>100</v>
       </c>
       <c r="G33" s="18">
@@ -4679,284 +4785,304 @@
       <c r="I33" s="19">
         <v>3</v>
       </c>
-      <c r="J33" s="25" t="s">
+      <c r="J33" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="K33" s="69" t="str">
+      <c r="K33" s="67">
         <f t="shared" ref="K33:K35" si="1">K34</f>
-        <v>-</v>
-      </c>
-      <c r="L33" s="152" t="s">
+        <v>1.4</v>
+      </c>
+      <c r="L33" s="150" t="s">
         <v>102</v>
       </c>
-      <c r="M33" s="153"/>
-      <c r="N33" s="152" t="s">
+      <c r="M33" s="151"/>
+      <c r="N33" s="150" t="s">
         <v>103</v>
       </c>
-      <c r="O33" s="153"/>
+      <c r="O33" s="151"/>
       <c r="P33" s="16"/>
-      <c r="XFA33" s="87" t="s">
+      <c r="XFA33" s="85" t="s">
         <v>120</v>
       </c>
-      <c r="XFB33" s="90" t="s">
+      <c r="XFB33" s="88" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="34" spans="2:16 16381:16383" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B34" s="51">
+      <c r="B34" s="49">
         <v>5</v>
       </c>
-      <c r="C34" s="122" t="s">
+      <c r="C34" s="120" t="s">
         <v>122</v>
       </c>
-      <c r="D34" s="144"/>
-      <c r="E34" s="145"/>
-      <c r="F34" s="34" t="str">
+      <c r="D34" s="225" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="226"/>
+      <c r="F34" s="32">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G34:$I34,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G34" s="97" t="str">
+        <v>1</v>
+      </c>
+      <c r="G34" s="95">
         <f>IF($D$34="Data or research outcomes cannot be used to directly identify data subjects or specific populations",1,"")</f>
-        <v/>
-      </c>
-      <c r="H34" s="101" t="str">
+        <v>1</v>
+      </c>
+      <c r="H34" s="99" t="str">
         <f>IF($D$34="Don’t know, or unsure if data or research outcomes could be used to directly identify data subjects",1,"")</f>
         <v/>
       </c>
-      <c r="I34" s="98" t="str">
+      <c r="I34" s="96" t="str">
         <f>IF($D$34="Data or research outcomes could directly identify data subjects or specific population groups",1,"")</f>
         <v/>
       </c>
-      <c r="J34" s="26"/>
-      <c r="K34" s="32" t="str">
+      <c r="J34" s="24"/>
+      <c r="K34" s="30">
         <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="L34" s="206" t="str">
+        <v>1.4</v>
+      </c>
+      <c r="L34" s="164" t="str">
         <f>IF($F$34=1,"Please explain the security arrangments that ensure direct identifcation is not possible",IF($F$34=2,"This selection has passed a tolerance. Please explain what actions will be taken to find out identifiability, and revise this item once known",IF($F$34=3,"This selection has passed a tolerance. Please explain why the data and research outcomes are identifiable and why this cannot be mitigated","Please select an option in cell D34")))</f>
-        <v>Please select an option in cell D34</v>
-      </c>
-      <c r="M34" s="207"/>
-      <c r="N34" s="210"/>
-      <c r="O34" s="211"/>
+        <v>Please explain the security arrangments that ensure direct identifcation is not possible</v>
+      </c>
+      <c r="M34" s="165"/>
+      <c r="N34" s="152" t="s">
+        <v>165</v>
+      </c>
+      <c r="O34" s="153"/>
       <c r="P34" s="16">
         <f>IF(SUM(H34:I34)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="XFA34" s="76" t="s">
+      <c r="XFA34" s="74" t="s">
         <v>123</v>
       </c>
-      <c r="XFB34" s="91" t="s">
+      <c r="XFB34" s="89" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="35" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B35" s="52">
+      <c r="B35" s="50">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C35" s="120" t="s">
+      <c r="C35" s="118" t="s">
         <v>125</v>
       </c>
-      <c r="D35" s="142"/>
-      <c r="E35" s="143"/>
-      <c r="F35" s="35" t="str">
+      <c r="D35" s="223" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" s="224"/>
+      <c r="F35" s="33">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G35:$I35,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G35" s="99" t="str">
+        <v>1</v>
+      </c>
+      <c r="G35" s="97">
         <f>IF($D$35="Data or research outcomes cannot be used indirectly to identify data subjects or specific population groups",1,"")</f>
-        <v/>
-      </c>
-      <c r="H35" s="101" t="str">
+        <v>1</v>
+      </c>
+      <c r="H35" s="99" t="str">
         <f>IF($D$35="Don’t know, or unsure if data or research outcomes could be used to indirectly identify data subjects",1,"")</f>
         <v/>
       </c>
-      <c r="I35" s="101" t="str">
+      <c r="I35" s="99" t="str">
         <f>IF($D$35="Data or research outcomes could indirectly identify data subjects or specific population groups",1,"")</f>
         <v/>
       </c>
-      <c r="J35" s="27"/>
-      <c r="K35" s="32" t="str">
+      <c r="J35" s="25"/>
+      <c r="K35" s="30">
         <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="L35" s="206" t="str">
+        <v>1.4</v>
+      </c>
+      <c r="L35" s="164" t="str">
         <f>IF($F$35=1,"Please explain the security arrangments that ensure indirect identifcation is not possible",IF($F$35=2,"This selection has passed a tolerance. Please explain what actions will be taken to find out identifiability, and revise this item once known",IF($F$35=3,"This selection has passed a tolerance. Please explain why the data and research outcomes are indirectly identifiable and why this cannot be mitigated","Please select an option in cell D35")))</f>
-        <v>Please select an option in cell D35</v>
-      </c>
-      <c r="M35" s="207"/>
-      <c r="N35" s="212"/>
-      <c r="O35" s="213"/>
+        <v>Please explain the security arrangments that ensure indirect identifcation is not possible</v>
+      </c>
+      <c r="M35" s="165"/>
+      <c r="N35" s="158" t="s">
+        <v>165</v>
+      </c>
+      <c r="O35" s="159"/>
       <c r="P35" s="16">
         <f>IF(SUM(H35:I35)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="XFA35" s="77"/>
-      <c r="XFB35" s="95" t="s">
+      <c r="XFA35" s="75"/>
+      <c r="XFB35" s="93" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="36" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B36" s="52">
+      <c r="B36" s="50">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C36" s="120" t="s">
+      <c r="C36" s="118" t="s">
         <v>127</v>
       </c>
-      <c r="D36" s="142"/>
-      <c r="E36" s="143"/>
-      <c r="F36" s="35" t="str">
+      <c r="D36" s="223" t="s">
+        <v>120</v>
+      </c>
+      <c r="E36" s="224"/>
+      <c r="F36" s="33">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G36:$I36,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G36" s="99" t="str">
+        <v>3</v>
+      </c>
+      <c r="G36" s="97" t="str">
         <f>IF($D$36="Strict data security in place to recognised standards that is proportionate to data use/sensitivity",1,"")</f>
         <v/>
       </c>
-      <c r="H36" s="112" t="str">
+      <c r="H36" s="110" t="str">
         <f>IF($D$36="Research taking place outside of a recognised secure environment, with proportionate data security precautions taken",1,"")</f>
         <v/>
       </c>
-      <c r="I36" s="101" t="str">
+      <c r="I36" s="99">
         <f>IF($D$36="Research taking place outside of a recognised secure environment, with some data security requirements still to be considered",1,"")</f>
-        <v/>
-      </c>
-      <c r="J36" s="27"/>
-      <c r="K36" s="32" t="str">
+        <v>1</v>
+      </c>
+      <c r="J36" s="25"/>
+      <c r="K36" s="30">
         <f>IFERROR(AVERAGE(F34:F38),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="L36" s="206" t="str">
+        <v>1.4</v>
+      </c>
+      <c r="L36" s="164" t="str">
         <f>IF($F$36=1,"Please state the secure research environment being used, and explain the data security arrangments in place",IF($F$36=2,"Please state the research environment being used, and what precautions are being taken to ensure data security",IF($F$36=3,"This selection has passed a tolerance. Please state the research environment being used, and what arrangements are still to be considered","Please select an option in cell D36")))</f>
-        <v>Please select an option in cell D36</v>
-      </c>
-      <c r="M36" s="207"/>
-      <c r="N36" s="214"/>
-      <c r="O36" s="215"/>
+        <v>This selection has passed a tolerance. Please state the research environment being used, and what arrangements are still to be considered</v>
+      </c>
+      <c r="M36" s="165"/>
+      <c r="N36" s="168" t="s">
+        <v>166</v>
+      </c>
+      <c r="O36" s="169"/>
       <c r="P36" s="16">
         <f>IF(SUM(I36)&gt;0, 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="XFA36" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="XFA36" s="76" t="s">
         <v>128</v>
       </c>
-      <c r="XFB36" s="83" t="s">
+      <c r="XFB36" s="81" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="37" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B37" s="52">
+      <c r="B37" s="50">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C37" s="123" t="s">
+      <c r="C37" s="121" t="s">
         <v>130</v>
       </c>
-      <c r="D37" s="142"/>
-      <c r="E37" s="143"/>
-      <c r="F37" s="35" t="str">
+      <c r="D37" s="223" t="s">
+        <v>128</v>
+      </c>
+      <c r="E37" s="224"/>
+      <c r="F37" s="33">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G37:$I37,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G37" s="99" t="str">
+        <v>1</v>
+      </c>
+      <c r="G37" s="97">
         <f>IF($D$37="Informed consent has been obtained from data subjects for all stages of this particular project.",1,"")</f>
-        <v/>
-      </c>
-      <c r="H37" s="112" t="str">
+        <v>1</v>
+      </c>
+      <c r="H37" s="110" t="str">
         <f>IF($D$37="Consent has not been obtained from data subjects for this particular research and can be justified",1,"")</f>
         <v/>
       </c>
-      <c r="I37" s="101" t="str">
+      <c r="I37" s="99" t="str">
         <f>IF($D$37="Informed consent has not been obtained from data subjects and cannot be justified",1,"")</f>
         <v/>
       </c>
-      <c r="J37" s="29"/>
-      <c r="K37" s="32" t="str">
+      <c r="J37" s="27"/>
+      <c r="K37" s="30">
         <f t="shared" ref="K37:K38" si="2">K36</f>
-        <v>-</v>
-      </c>
-      <c r="L37" s="206" t="str">
+        <v>1.4</v>
+      </c>
+      <c r="L37" s="164" t="str">
         <f>IF($F$37=1,"Please explain the measures in place to gain fully informed consent for this project",IF($F$37=2,"Please provide a justification as to why ethcial consent is not being sought for this particular project?",IF($F$37=3,"This selection has passed a tolerance. Please explain why consent is not being sought","Please select an option in cell D37")))</f>
-        <v>Please select an option in cell D37</v>
-      </c>
-      <c r="M37" s="207"/>
-      <c r="N37" s="229"/>
-      <c r="O37" s="230"/>
+        <v>Please explain the measures in place to gain fully informed consent for this project</v>
+      </c>
+      <c r="M37" s="165"/>
+      <c r="N37" s="154" t="s">
+        <v>167</v>
+      </c>
+      <c r="O37" s="155"/>
       <c r="P37" s="16">
         <f>IF(SUM(I37)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="XFA37" s="78" t="s">
+      <c r="XFA37" s="76" t="s">
         <v>131</v>
       </c>
-      <c r="XFB37" s="83" t="s">
+      <c r="XFB37" s="81" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="38" spans="2:16 16381:16383" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B38" s="53">
+      <c r="B38" s="51">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C38" s="121" t="s">
+      <c r="C38" s="119" t="s">
         <v>133</v>
       </c>
-      <c r="D38" s="146"/>
-      <c r="E38" s="147"/>
-      <c r="F38" s="36" t="str">
+      <c r="D38" s="227" t="s">
+        <v>138</v>
+      </c>
+      <c r="E38" s="228"/>
+      <c r="F38" s="34">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G38:$I38,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G38" s="106" t="str">
+        <v>1</v>
+      </c>
+      <c r="G38" s="104">
         <f>IF($D$38="Permission has been given specifically for this research project, or the proposed use of data is within the same context for which permission was previously given",1,"")</f>
-        <v/>
-      </c>
-      <c r="H38" s="108" t="str">
+        <v>1</v>
+      </c>
+      <c r="H38" s="106" t="str">
         <f>IF($D$38="Don’t know, or unsure if the proposed use of data is beyond the initial context for which permission was originally given",1,"")</f>
         <v/>
       </c>
-      <c r="I38" s="108" t="str">
+      <c r="I38" s="106" t="str">
         <f>IF($D$38="The proposed use of data is beyond the initial context for which permission was originally given",1,"")</f>
         <v/>
       </c>
-      <c r="J38" s="109" t="str">
+      <c r="J38" s="107" t="str">
         <f>IF($D$38="N/A: Omit this item when permission to access data is not required",1,"")</f>
         <v/>
       </c>
-      <c r="K38" s="33" t="str">
+      <c r="K38" s="31">
         <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-      <c r="L38" s="206" t="str">
+        <v>1.4</v>
+      </c>
+      <c r="L38" s="164" t="str">
         <f>IF($F$38=1,"Please outline the permissions that are in place",IF($F$38=2,"This selection has passed a tolerance. Please seek clarity on this issue",IF($F$38=3,"This selection has passed a tolerance. Please explain how you are going to ensure any outstanding data owner permissions are secured",IF($J$38=1,"In instances where permission is not needed, please provide a solid justification, along with evidence, to explain why permission is not required","Please select an option in cell D38"))))</f>
-        <v>Please select an option in cell D38</v>
-      </c>
-      <c r="M38" s="207"/>
-      <c r="N38" s="212"/>
-      <c r="O38" s="213"/>
+        <v>Please outline the permissions that are in place</v>
+      </c>
+      <c r="M38" s="165"/>
+      <c r="N38" s="158" t="s">
+        <v>168</v>
+      </c>
+      <c r="O38" s="159"/>
       <c r="P38" s="16">
         <f>IF(SUM(H38:I38)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="XFA38" s="79" t="s">
+      <c r="XFA38" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="XFB38" s="87" t="s">
+      <c r="XFB38" s="85" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="39" spans="2:16 16381:16383" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="20"/>
-      <c r="C39" s="56" t="s">
+      <c r="C39" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="D39" s="161" t="s">
+      <c r="D39" s="174" t="s">
         <v>99</v>
       </c>
-      <c r="E39" s="160"/>
-      <c r="F39" s="37" t="s">
+      <c r="E39" s="175"/>
+      <c r="F39" s="35" t="s">
         <v>100</v>
       </c>
       <c r="G39" s="18">
@@ -4968,297 +5094,321 @@
       <c r="I39" s="19">
         <v>3</v>
       </c>
-      <c r="J39" s="25" t="s">
+      <c r="J39" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="K39" s="69" t="str">
+      <c r="K39" s="67">
         <f t="shared" ref="K39:K41" si="3">K40</f>
-        <v>-</v>
-      </c>
-      <c r="L39" s="152" t="s">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="L39" s="150" t="s">
         <v>102</v>
       </c>
-      <c r="M39" s="153"/>
-      <c r="N39" s="152" t="s">
+      <c r="M39" s="151"/>
+      <c r="N39" s="150" t="s">
         <v>103</v>
       </c>
-      <c r="O39" s="153"/>
+      <c r="O39" s="151"/>
       <c r="P39" s="16"/>
-      <c r="XFA39" s="88" t="s">
+      <c r="XFA39" s="86" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="40" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B40" s="51">
+      <c r="B40" s="49">
         <v>10</v>
       </c>
-      <c r="C40" s="122" t="s">
+      <c r="C40" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="148"/>
-      <c r="E40" s="149"/>
-      <c r="F40" s="34" t="str">
+      <c r="D40" s="229" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="230"/>
+      <c r="F40" s="32">
         <f t="shared" ref="F40:F45" si="4">IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G40:$I40,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G40" s="97" t="str">
+        <v>1</v>
+      </c>
+      <c r="G40" s="95">
         <f>IF($D$40="Confidence that the methods used, and quality of data will lead to valid conclusions",1,"")</f>
-        <v/>
-      </c>
-      <c r="H40" s="110" t="str">
+        <v>1</v>
+      </c>
+      <c r="H40" s="108" t="str">
         <f>IF($D$40="There is limited confidence/it is unsure whether the methods used, and quality of data will lead to valid conclusions",1,"")</f>
         <v/>
       </c>
-      <c r="I40" s="98" t="str">
+      <c r="I40" s="96" t="str">
         <f>IF($D$40="Potential that methods used, and quality of data may/will lead to invalid conclusions",1,"")</f>
         <v/>
       </c>
-      <c r="J40" s="26"/>
-      <c r="K40" s="32" t="str">
+      <c r="J40" s="24"/>
+      <c r="K40" s="30">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="L40" s="206" t="str">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="L40" s="164" t="str">
         <f>IF($F$40=1,"Please explain why methods and data used will confidently lead to valid conclusions",IF($F$40=2,"Please explain why you have limited confidence/are unsure whether methods and data used will lead to valid conclusions, and provide mitigations against this uncertainty",IF($F$40=3,"This selection has passed a tolerance. Please explain why methods and data used may lead to invalid conclusions, justify the use of these methods or data, and provide any mitigations","Please select an option in cell D40")))</f>
-        <v>Please select an option in cell D40</v>
-      </c>
-      <c r="M40" s="207"/>
-      <c r="N40" s="210"/>
-      <c r="O40" s="211"/>
+        <v>Please explain why methods and data used will confidently lead to valid conclusions</v>
+      </c>
+      <c r="M40" s="165"/>
+      <c r="N40" s="152" t="s">
+        <v>169</v>
+      </c>
+      <c r="O40" s="153"/>
       <c r="P40" s="16">
         <f>IF(SUM(I40:I40)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="XFA40" s="88" t="s">
+      <c r="XFA40" s="86" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="41" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B41" s="52">
+      <c r="B41" s="50">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C41" s="123" t="s">
+      <c r="C41" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="150"/>
-      <c r="E41" s="151"/>
-      <c r="F41" s="35" t="str">
+      <c r="D41" s="170" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="171"/>
+      <c r="F41" s="33">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="G41" s="99" t="str">
+        <v>1</v>
+      </c>
+      <c r="G41" s="97">
         <f>IF($D$41="The research organisation has established and tested procedures, and complies with recognised standards",1,"")</f>
-        <v/>
-      </c>
-      <c r="H41" s="112" t="str">
+        <v>1</v>
+      </c>
+      <c r="H41" s="110" t="str">
         <f>IF($D$41="There is limited confidence/it is not clear whether the organisation has established and tested procedures, and complies with recognised standards",1,"")</f>
         <v/>
       </c>
-      <c r="I41" s="101" t="str">
+      <c r="I41" s="99" t="str">
         <f>IF($D$41="The research organisation does not have established clear procedures or may not comply with recognised standards",1,"")</f>
         <v/>
       </c>
-      <c r="J41" s="27"/>
-      <c r="K41" s="32" t="str">
+      <c r="J41" s="25"/>
+      <c r="K41" s="30">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="L41" s="206" t="str">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="L41" s="164" t="str">
         <f>IF($F$41=1,"Please explain the established research standards of the research organisation",IF($F$41=2,"Please explain why you have limited confidence/are unsure whether the organisation has established procedures",IF($F$41=3,"This selection has passed a tolerance. Please provide mitigations for this risk, and explain why research is to be done without clear and compliant procedures","Please select an option in cell D41")))</f>
-        <v>Please select an option in cell D41</v>
-      </c>
-      <c r="M41" s="207"/>
-      <c r="N41" s="229"/>
-      <c r="O41" s="230"/>
+        <v>Please explain the established research standards of the research organisation</v>
+      </c>
+      <c r="M41" s="165"/>
+      <c r="N41" s="158" t="s">
+        <v>168</v>
+      </c>
+      <c r="O41" s="159"/>
       <c r="P41" s="16">
         <f>IF(SUM(I41)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="XFA41" s="83" t="s">
+      <c r="XFA41" s="81" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="42" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B42" s="52">
+      <c r="B42" s="50">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C42" s="120" t="s">
+      <c r="C42" s="118" t="s">
         <v>35</v>
       </c>
-      <c r="D42" s="150"/>
-      <c r="E42" s="151"/>
-      <c r="F42" s="35" t="str">
+      <c r="D42" s="170" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="171"/>
+      <c r="F42" s="33">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="G42" s="99" t="str">
+        <v>1</v>
+      </c>
+      <c r="G42" s="97">
         <f>IF($D$42="Researchers are appropriately trained to recognised standards",1,"")</f>
-        <v/>
-      </c>
-      <c r="H42" s="100" t="str">
+        <v>1</v>
+      </c>
+      <c r="H42" s="98" t="str">
         <f>IF($D$42="Researchers are trained but have limited experience in particular research area",1,"")</f>
         <v/>
       </c>
-      <c r="I42" s="101" t="str">
+      <c r="I42" s="99" t="str">
         <f>IF($D$42="Researchers are trained but there is limited assurance in training that relates to this research",1,"")</f>
         <v/>
       </c>
-      <c r="J42" s="27"/>
-      <c r="K42" s="32" t="str">
+      <c r="J42" s="25"/>
+      <c r="K42" s="30">
         <f>IFERROR(AVERAGE(F40:F45),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="L42" s="206" t="str">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="L42" s="164" t="str">
         <f>IF($F$42=1,"Please explain the training that researchers have received to do this research",IF($F$42=2,"Please explain why researchers are to be used with limited training, and provide a mitigation agasint this limitation",IF($F$42=3,"This selection has passed a tolerance. Please explain the training that has been recieved, and why there is limited assurance that it relates to this research","Please select an option in cell D42")))</f>
-        <v>Please select an option in cell D42</v>
-      </c>
-      <c r="M42" s="207"/>
-      <c r="N42" s="212"/>
-      <c r="O42" s="213"/>
+        <v>Please explain the training that researchers have received to do this research</v>
+      </c>
+      <c r="M42" s="165"/>
+      <c r="N42" s="158" t="s">
+        <v>171</v>
+      </c>
+      <c r="O42" s="159"/>
       <c r="P42" s="16">
         <f>IF(SUM(I42:I42)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="XFA42" s="83" t="s">
+      <c r="XFA42" s="81" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="43" spans="2:16 16381:16383" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B43" s="52">
+      <c r="B43" s="50">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C43" s="120" t="s">
+      <c r="C43" s="118" t="s">
         <v>141</v>
       </c>
-      <c r="D43" s="150"/>
-      <c r="E43" s="151"/>
-      <c r="F43" s="35" t="str">
+      <c r="D43" s="170" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="171"/>
+      <c r="F43" s="33">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="G43" s="99" t="str">
+        <v>1</v>
+      </c>
+      <c r="G43" s="97">
         <f>IF($D$43="Human oversight of all elements of research process, and regular audits of automated outcomes",1,"")</f>
-        <v/>
-      </c>
-      <c r="H43" s="100" t="str">
+        <v>1</v>
+      </c>
+      <c r="H43" s="98" t="str">
         <f>IF($D$43="Significant use of automated processes and/or off the shelf solutions with some level of human oversight",1,"")</f>
         <v/>
       </c>
-      <c r="I43" s="101" t="str">
+      <c r="I43" s="99" t="str">
         <f>IF($D$43="Research based on automated or opaque processes with minimal human oversight",1,"")</f>
         <v/>
       </c>
-      <c r="J43" s="102" t="str">
+      <c r="J43" s="100" t="str">
         <f>IF($D$43="N/A: Omit this item in case of fully transparent automated or manual processes with well documented assumptions",1,"")</f>
         <v/>
       </c>
-      <c r="K43" s="32" t="str">
+      <c r="K43" s="30">
         <f t="shared" ref="K43:K45" si="5">K42</f>
-        <v>-</v>
-      </c>
-      <c r="L43" s="206" t="str">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="L43" s="164" t="str">
         <f>IF($F$43=1,"Please explain the planned human oversight processes for this project",IF($F$43=2,"Please explain the level of human oversight, and explain why it is limited",IF($F$43=3,"This selection has passed a tolerance. Please explain why there is minimal human oversight and provide a mitigation for this",IF($J$43=1,"Please justify the omission of this item","Please select an option in cell D43"))))</f>
-        <v>Please select an option in cell D43</v>
-      </c>
-      <c r="M43" s="207"/>
-      <c r="N43" s="229"/>
-      <c r="O43" s="230"/>
+        <v>Please explain the planned human oversight processes for this project</v>
+      </c>
+      <c r="M43" s="165"/>
+      <c r="N43" s="154" t="s">
+        <v>170</v>
+      </c>
+      <c r="O43" s="155"/>
       <c r="P43" s="16">
         <f>IF(SUM(I43:I43)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="XFA43" s="87" t="s">
+      <c r="XFA43" s="85" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="44" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B44" s="52">
+      <c r="B44" s="50">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C44" s="123" t="s">
+      <c r="C44" s="121" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="150"/>
-      <c r="E44" s="151"/>
-      <c r="F44" s="35" t="str">
+      <c r="D44" s="170" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" s="171"/>
+      <c r="F44" s="33">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="G44" s="99" t="str">
+        <v>1</v>
+      </c>
+      <c r="G44" s="97">
         <f>IF($D$44="Research utilises well established methods and technologies",1,"")</f>
-        <v/>
-      </c>
-      <c r="H44" s="100" t="str">
+        <v>1</v>
+      </c>
+      <c r="H44" s="98" t="str">
         <f>IF($D$44="Methods and tools may be tried, but are still novel or automated",1,"")</f>
         <v/>
       </c>
-      <c r="I44" s="101" t="str">
+      <c r="I44" s="99" t="str">
         <f>IF($D$44="Research utilises untested or automated methods and technologies",1,"")</f>
         <v/>
       </c>
-      <c r="J44" s="102" t="str">
+      <c r="J44" s="100" t="str">
         <f>IF($D$44="N/A: Omit this item for small-scale exploratory projects and feasibility studies which are not used to produce any research/statistical outputs",1,"")</f>
         <v/>
       </c>
-      <c r="K44" s="32" t="str">
+      <c r="K44" s="30">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="L44" s="206" t="str">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="L44" s="164" t="str">
         <f>IF($F$44=1,"Please briefly outline the standard methods and technologies used",IF($F$44=2,"Please justify the use of this method, and provide mitigations against the risk of automation and/or using novel methods",IF($F$44=3,"This selection has passed a tolerance. Please justify the use of this method/tool, and provide mitigations",IF($J$44=1,"Please justify the omission of this item","Please select an option in cell D44"))))</f>
-        <v>Please select an option in cell D44</v>
-      </c>
-      <c r="M44" s="207"/>
-      <c r="N44" s="229"/>
-      <c r="O44" s="230"/>
-      <c r="P44" s="116">
+        <v>Please briefly outline the standard methods and technologies used</v>
+      </c>
+      <c r="M44" s="165"/>
+      <c r="N44" s="154" t="s">
+        <v>172</v>
+      </c>
+      <c r="O44" s="155"/>
+      <c r="P44" s="114">
         <f>IF(SUM(I44)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="XFC44" s="64"/>
+      <c r="XFC44" s="62"/>
     </row>
     <row r="45" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B45" s="53">
+      <c r="B45" s="51">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C45" s="124" t="s">
+      <c r="C45" s="122" t="s">
         <v>95</v>
       </c>
-      <c r="D45" s="157"/>
-      <c r="E45" s="158"/>
-      <c r="F45" s="36" t="str">
+      <c r="D45" s="172" t="s">
+        <v>109</v>
+      </c>
+      <c r="E45" s="173"/>
+      <c r="F45" s="34">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="G45" s="106" t="str">
+        <v>2</v>
+      </c>
+      <c r="G45" s="104" t="str">
         <f>IF($D$45="Methods and quality of data will most likely result in realising the research benefits and fully mitigate any risks",1,"")</f>
         <v/>
       </c>
-      <c r="H45" s="111" t="str">
+      <c r="H45" s="109">
         <f>IF($D$45="There is limited confidence/it is unsure whether the methods and quality of data will result in realising research benefits or mitigate risks",1,"")</f>
-        <v/>
-      </c>
-      <c r="I45" s="108" t="str">
+        <v>1</v>
+      </c>
+      <c r="I45" s="106" t="str">
         <f>IF($D$45="Methods and quality of data have little/no potential to result in realising research benefits or mitigate risks",1,"")</f>
         <v/>
       </c>
-      <c r="J45" s="28"/>
-      <c r="K45" s="33" t="str">
+      <c r="J45" s="26"/>
+      <c r="K45" s="31">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="L45" s="206" t="str">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="L45" s="164" t="str">
         <f>IF($F$45=1,"Please justify your confidence that the public good will be realised",IF($F$45=2,"Please explain why there is limited confidence/it is unsure that the public good will be realised, and justify why research should occur nonetheless",IF($F$45=3,"This selection has passed a tolerance. Please explain why the methods and data are still being pursued if there is little/no chance of the public good being realised","Please select an option in cell D45")))</f>
-        <v>Please select an option in cell D45</v>
-      </c>
-      <c r="M45" s="207"/>
-      <c r="N45" s="233"/>
-      <c r="O45" s="234"/>
+        <v>Please explain why there is limited confidence/it is unsure that the public good will be realised, and justify why research should occur nonetheless</v>
+      </c>
+      <c r="M45" s="165"/>
+      <c r="N45" s="160" t="s">
+        <v>173</v>
+      </c>
+      <c r="O45" s="161"/>
       <c r="P45" s="16">
         <f>IF(SUM(I45:I45)&gt;0, 1, 0)</f>
         <v>0</v>
@@ -5266,14 +5416,14 @@
     </row>
     <row r="46" spans="2:16 16381:16383" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" s="20"/>
-      <c r="C46" s="39" t="s">
+      <c r="C46" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="D46" s="161" t="s">
+      <c r="D46" s="174" t="s">
         <v>99</v>
       </c>
-      <c r="E46" s="160"/>
-      <c r="F46" s="37" t="s">
+      <c r="E46" s="175"/>
+      <c r="F46" s="35" t="s">
         <v>100</v>
       </c>
       <c r="G46" s="18">
@@ -5285,103 +5435,111 @@
       <c r="I46" s="19">
         <v>3</v>
       </c>
-      <c r="J46" s="25" t="s">
+      <c r="J46" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="K46" s="32" t="str">
+      <c r="K46" s="30">
         <f>K47</f>
-        <v>-</v>
-      </c>
-      <c r="L46" s="152" t="s">
+        <v>1</v>
+      </c>
+      <c r="L46" s="150" t="s">
         <v>102</v>
       </c>
-      <c r="M46" s="153"/>
-      <c r="N46" s="152" t="s">
+      <c r="M46" s="151"/>
+      <c r="N46" s="150" t="s">
         <v>103</v>
       </c>
-      <c r="O46" s="153"/>
-      <c r="P46" s="117"/>
+      <c r="O46" s="151"/>
+      <c r="P46" s="115"/>
     </row>
     <row r="47" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B47" s="51">
+      <c r="B47" s="49">
         <v>16</v>
       </c>
-      <c r="C47" s="125" t="s">
+      <c r="C47" s="123" t="s">
         <v>144</v>
       </c>
-      <c r="D47" s="144"/>
-      <c r="E47" s="145"/>
-      <c r="F47" s="34" t="str">
+      <c r="D47" s="225" t="s">
+        <v>118</v>
+      </c>
+      <c r="E47" s="226"/>
+      <c r="F47" s="32">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G47:$I47,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G47" s="97" t="str">
+        <v>1</v>
+      </c>
+      <c r="G47" s="95">
         <f>IF($D$47="The proposed use of data has been cleared against all relevant legislation and agreements",1,"")</f>
-        <v/>
-      </c>
-      <c r="H47" s="98" t="str">
+        <v>1</v>
+      </c>
+      <c r="H47" s="96" t="str">
         <f>IF($D$47="Don’t know, or unsure if the proposed use of data has been cleared against all relevant legislation and agreements",1,"")</f>
         <v/>
       </c>
-      <c r="I47" s="98" t="str">
+      <c r="I47" s="96" t="str">
         <f>IF($D$47="Legality has not been confirmed, and/or there has been no formal action to seek legal advice or clearance from the relevant department",1,"")</f>
         <v/>
       </c>
-      <c r="J47" s="26"/>
-      <c r="K47" s="31" t="str">
+      <c r="J47" s="24"/>
+      <c r="K47" s="29">
         <f>IFERROR(AVERAGE(F47:F48),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="L47" s="204" t="str">
+        <v>1</v>
+      </c>
+      <c r="L47" s="187" t="str">
         <f>IF($F$47=1,"Which legal gateways are required to facilitate this research? You may wish to consult the guidance document.",IF($F$47=2,"This selection has passed a tolerance. Please consult with available legal services support to confirm",IF($F$47=3,"This selection has passed a tolerance. Legality must be confirmed, please consult with available legal services support before proceeding","Please select an option in cell D47")))</f>
-        <v>Please select an option in cell D47</v>
-      </c>
-      <c r="M47" s="205"/>
-      <c r="N47" s="210"/>
-      <c r="O47" s="211"/>
-      <c r="P47" s="116">
+        <v>Which legal gateways are required to facilitate this research? You may wish to consult the guidance document.</v>
+      </c>
+      <c r="M47" s="188"/>
+      <c r="N47" s="152" t="s">
+        <v>168</v>
+      </c>
+      <c r="O47" s="153"/>
+      <c r="P47" s="114">
         <f>IF(SUM(H47:I47)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:16 16381:16383" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B48" s="53">
+      <c r="B48" s="51">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C48" s="126" t="s">
+      <c r="C48" s="124" t="s">
         <v>145</v>
       </c>
-      <c r="D48" s="146"/>
-      <c r="E48" s="147"/>
-      <c r="F48" s="36" t="str">
+      <c r="D48" s="227" t="s">
+        <v>129</v>
+      </c>
+      <c r="E48" s="228"/>
+      <c r="F48" s="34">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G48:$I48,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G48" s="106" t="str">
+        <v>1</v>
+      </c>
+      <c r="G48" s="104">
         <f>IF($D$48="Legal frameworks are clear and well established in the research area",1,"")</f>
-        <v/>
-      </c>
-      <c r="H48" s="108" t="str">
+        <v>1</v>
+      </c>
+      <c r="H48" s="106" t="str">
         <f>IF($D$48="Don’t know, or unsure what the relevant legal frameworks are in the research area",1,"")</f>
         <v/>
       </c>
-      <c r="I48" s="108" t="str">
+      <c r="I48" s="106" t="str">
         <f>IF($D$48="Legal frameworks are unclear or still developing in the research area",1,"")</f>
         <v/>
       </c>
-      <c r="J48" s="26"/>
-      <c r="K48" s="32" t="str">
+      <c r="J48" s="24"/>
+      <c r="K48" s="30">
         <f>K47</f>
-        <v>-</v>
-      </c>
-      <c r="L48" s="202" t="str">
+        <v>1</v>
+      </c>
+      <c r="L48" s="185" t="str">
         <f>IF($F$48=1,"Which are the legal frameworks pertinent to this project? You may wish to consult the guidance document.",IF($F$48=2,"This selection has passed a tolerance. Please consult with available legal services support to conflrm",IF($F$48=3,"This selection has passed a tolerance. Legality must be confirmed, please consult with available legal services support before proceeding","Please select an option in cell D48")))</f>
-        <v>Please select an option in cell D48</v>
-      </c>
-      <c r="M48" s="203"/>
-      <c r="N48" s="212"/>
-      <c r="O48" s="213"/>
+        <v>Which are the legal frameworks pertinent to this project? You may wish to consult the guidance document.</v>
+      </c>
+      <c r="M48" s="186"/>
+      <c r="N48" s="158" t="s">
+        <v>168</v>
+      </c>
+      <c r="O48" s="159"/>
       <c r="P48" s="16">
         <f>IF(SUM(H48:I48)&gt;0, 1, 0)</f>
         <v>0</v>
@@ -5389,14 +5547,14 @@
     </row>
     <row r="49" spans="2:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" s="20"/>
-      <c r="C49" s="56" t="s">
+      <c r="C49" s="54" t="s">
         <v>146</v>
       </c>
-      <c r="D49" s="161" t="s">
+      <c r="D49" s="174" t="s">
         <v>99</v>
       </c>
-      <c r="E49" s="160"/>
-      <c r="F49" s="37" t="s">
+      <c r="E49" s="175"/>
+      <c r="F49" s="35" t="s">
         <v>100</v>
       </c>
       <c r="G49" s="18">
@@ -5408,121 +5566,129 @@
       <c r="I49" s="19">
         <v>3</v>
       </c>
-      <c r="J49" s="25" t="s">
+      <c r="J49" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="K49" s="69" t="str">
+      <c r="K49" s="67">
         <f>K50</f>
-        <v>-</v>
-      </c>
-      <c r="L49" s="152" t="s">
+        <v>3</v>
+      </c>
+      <c r="L49" s="150" t="s">
         <v>102</v>
       </c>
-      <c r="M49" s="153"/>
-      <c r="N49" s="152" t="s">
+      <c r="M49" s="151"/>
+      <c r="N49" s="150" t="s">
         <v>103</v>
       </c>
-      <c r="O49" s="153"/>
+      <c r="O49" s="151"/>
       <c r="P49" s="16"/>
     </row>
-    <row r="50" spans="2:16" ht="120" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B50" s="54">
+    <row r="50" spans="2:16" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50" s="52">
         <v>18</v>
       </c>
-      <c r="C50" s="122" t="s">
+      <c r="C50" s="120" t="s">
         <v>147</v>
       </c>
-      <c r="D50" s="148"/>
-      <c r="E50" s="149"/>
-      <c r="F50" s="34" t="str">
+      <c r="D50" s="229" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="230"/>
+      <c r="F50" s="32">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G50:$I50,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G50" s="97" t="str">
+        <v>3</v>
+      </c>
+      <c r="G50" s="95" t="str">
         <f>IF($D$50="The public is widely supportive of the project aim and  method",1,"")</f>
         <v/>
       </c>
-      <c r="H50" s="113" t="str">
+      <c r="H50" s="111" t="str">
         <f>IF($D$50="There is limited support of the project aim and methods from the public",1,"")</f>
         <v/>
       </c>
-      <c r="I50" s="98" t="str">
+      <c r="I50" s="96">
         <f>IF($D$50="The public’s views of the project aims, and method are negative or unknown",1,"")</f>
-        <v/>
-      </c>
-      <c r="J50" s="26"/>
-      <c r="K50" s="32" t="str">
+        <v>1</v>
+      </c>
+      <c r="J50" s="24"/>
+      <c r="K50" s="30">
         <f>IFERROR(AVERAGE(F50:F51), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="L50" s="204" t="str">
+        <v>3</v>
+      </c>
+      <c r="L50" s="187" t="str">
         <f>IF($F$50=1,"Please explain the positive public views, and evidence how this is known",IF($F$50=2,"Please explain the limited public support, evidence how this is known, and provide a mitigation",IF($F$50=3,"This selection has passed a tolerance. Either explain and justify why the views are unknown or explain the public's negative views, and evidence how this is known","Please select an option in cell D50")))</f>
-        <v>Please select an option in cell D50</v>
-      </c>
-      <c r="M50" s="205"/>
-      <c r="N50" s="210"/>
-      <c r="O50" s="211"/>
+        <v>This selection has passed a tolerance. Either explain and justify why the views are unknown or explain the public's negative views, and evidence how this is known</v>
+      </c>
+      <c r="M50" s="188"/>
+      <c r="N50" s="152" t="s">
+        <v>174</v>
+      </c>
+      <c r="O50" s="153"/>
       <c r="P50" s="16">
         <f>IF(SUM(I50)&gt;0, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="2:16" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B51" s="53">
+      <c r="B51" s="51">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C51" s="121" t="s">
+      <c r="C51" s="119" t="s">
         <v>21</v>
       </c>
-      <c r="D51" s="157"/>
-      <c r="E51" s="158"/>
-      <c r="F51" s="36" t="str">
+      <c r="D51" s="172" t="s">
+        <v>33</v>
+      </c>
+      <c r="E51" s="173"/>
+      <c r="F51" s="34">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G51:$I51,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G51" s="106" t="str">
+        <v>3</v>
+      </c>
+      <c r="G51" s="104" t="str">
         <f>IF($D$51="The research involves regular engagement with the public and/or stakeholders",1,"")</f>
         <v/>
       </c>
-      <c r="H51" s="107" t="str">
+      <c r="H51" s="105" t="str">
         <f>IF($D$51="The research involves some engagement, though it is not regular throughout the research project",1,"")</f>
         <v/>
       </c>
-      <c r="I51" s="108" t="str">
+      <c r="I51" s="106">
         <f>IF($D$51="No public engagement has been conducted, or planned, as part of the project",1,"")</f>
-        <v/>
-      </c>
-      <c r="J51" s="109" t="str">
+        <v>1</v>
+      </c>
+      <c r="J51" s="107" t="str">
         <f>IF($D$51="N/A: Omit this item when no public engagement is required and can be clearly justified",1,"")</f>
         <v/>
       </c>
-      <c r="K51" s="32" t="str">
+      <c r="K51" s="30">
         <f>K50</f>
-        <v>-</v>
-      </c>
-      <c r="L51" s="206" t="str">
+        <v>3</v>
+      </c>
+      <c r="L51" s="164" t="str">
         <f>IF($F$51=1,"Please outline the planned regular public engagement",IF($F$51=2,"Please outline the engagement planned, and justify why it is not regular throughout the project",IF($F$51=3,"This selection has passed a tolerance. Please explain and justify why no public engagement is planned or required",IF($J$51=1,"Please explain why public engagment is not needed for this project","Please select an option in cell D51"))))</f>
-        <v>Please select an option in cell D51</v>
-      </c>
-      <c r="M51" s="207"/>
-      <c r="N51" s="231"/>
-      <c r="O51" s="232"/>
+        <v>This selection has passed a tolerance. Please explain and justify why no public engagement is planned or required</v>
+      </c>
+      <c r="M51" s="165"/>
+      <c r="N51" s="152" t="s">
+        <v>175</v>
+      </c>
+      <c r="O51" s="153"/>
       <c r="P51" s="16">
         <f>IF(SUM(I51)&gt;0, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="2:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B52" s="21"/>
-      <c r="C52" s="56" t="s">
+      <c r="C52" s="54" t="s">
         <v>148</v>
       </c>
-      <c r="D52" s="161" t="s">
+      <c r="D52" s="174" t="s">
         <v>99</v>
       </c>
-      <c r="E52" s="160"/>
-      <c r="F52" s="37" t="s">
+      <c r="E52" s="175"/>
+      <c r="F52" s="35" t="s">
         <v>100</v>
       </c>
       <c r="G52" s="18">
@@ -5534,210 +5700,310 @@
       <c r="I52" s="19">
         <v>3</v>
       </c>
-      <c r="J52" s="25" t="s">
+      <c r="J52" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="K52" s="31" t="str">
+      <c r="K52" s="29">
         <f>K53</f>
-        <v>-</v>
-      </c>
-      <c r="L52" s="152" t="s">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="L52" s="150" t="s">
         <v>102</v>
       </c>
-      <c r="M52" s="153"/>
-      <c r="N52" s="152" t="s">
+      <c r="M52" s="151"/>
+      <c r="N52" s="150" t="s">
         <v>103</v>
       </c>
-      <c r="O52" s="153"/>
+      <c r="O52" s="151"/>
       <c r="P52" s="16"/>
     </row>
     <row r="53" spans="2:16" ht="120" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B53" s="51">
+      <c r="B53" s="49">
         <v>20</v>
       </c>
-      <c r="C53" s="125" t="s">
+      <c r="C53" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="D53" s="144"/>
-      <c r="E53" s="145"/>
-      <c r="F53" s="34" t="str">
+      <c r="D53" s="225" t="s">
+        <v>47</v>
+      </c>
+      <c r="E53" s="226"/>
+      <c r="F53" s="32">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G53:$I53,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G53" s="97" t="str">
+        <v>2</v>
+      </c>
+      <c r="G53" s="95" t="str">
         <f>IF($D$53="Research outcomes are,or will be, openly available to the public",1,"")</f>
         <v/>
       </c>
-      <c r="H53" s="98" t="str">
+      <c r="H53" s="96">
         <f>IF($D$53="Don’t know, or unsure if research outcomes will be openly available to the public",1,"")</f>
-        <v/>
-      </c>
-      <c r="I53" s="98" t="str">
+        <v>1</v>
+      </c>
+      <c r="I53" s="96" t="str">
         <f>IF($D$53="Research outcomes are not, or will not be, openly available to the public",1,"")</f>
         <v/>
       </c>
-      <c r="J53" s="30"/>
-      <c r="K53" s="31" t="str">
+      <c r="J53" s="28"/>
+      <c r="K53" s="29">
         <f>IFERROR(AVERAGE(F53:F55),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="L53" s="204" t="str">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="L53" s="187" t="str">
         <f>IF($F$53=1,"Please explain how research outcomes will be made openly available to the public",IF($F$53=2,"This selection has passed a tolerance. Please explain why the potential for public access to outcomes is unknown",IF($F$53=3,"This selection has passed a tolerance. Please explain why outcomes will not be openly available to the public","Please select an option in cell D53")))</f>
-        <v>Please select an option in cell D53</v>
-      </c>
-      <c r="M53" s="205"/>
-      <c r="N53" s="210"/>
-      <c r="O53" s="211"/>
+        <v>This selection has passed a tolerance. Please explain why the potential for public access to outcomes is unknown</v>
+      </c>
+      <c r="M53" s="188"/>
+      <c r="N53" s="152" t="s">
+        <v>178</v>
+      </c>
+      <c r="O53" s="153"/>
       <c r="P53" s="16">
         <f>IF(SUM(H53:I53)&gt;0, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="2:16" ht="120" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B54" s="52">
+      <c r="B54" s="50">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C54" s="127" t="s">
+      <c r="C54" s="125" t="s">
         <v>149</v>
       </c>
-      <c r="D54" s="150"/>
-      <c r="E54" s="151"/>
-      <c r="F54" s="35" t="str">
+      <c r="D54" s="170" t="s">
+        <v>66</v>
+      </c>
+      <c r="E54" s="171"/>
+      <c r="F54" s="33">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G54:$I54,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G54" s="99" t="str">
+        <v>2</v>
+      </c>
+      <c r="G54" s="97" t="str">
         <f>IF($D$54="Both methods and/or tools are, or will be, made widely available to the public",1,"")</f>
         <v/>
       </c>
-      <c r="H54" s="100" t="str">
+      <c r="H54" s="98">
         <f>IF($D$54="Don’t know, or unsure if methods and tools will be available to the public",1,"")</f>
-        <v/>
-      </c>
-      <c r="I54" s="101" t="str">
+        <v>1</v>
+      </c>
+      <c r="I54" s="99" t="str">
         <f>IF($D$54="Both methods and tools are not, or will not be, made widely available to the public, or will only be shared internally",1,"")</f>
         <v/>
       </c>
-      <c r="J54" s="102" t="str">
+      <c r="J54" s="100" t="str">
         <f>IF($D$54="N/A: Omit this item when you are not able to share these tools and methods",1,"")</f>
         <v/>
       </c>
-      <c r="K54" s="32" t="str">
+      <c r="K54" s="30">
         <f t="shared" ref="K54:K55" si="6">K53</f>
-        <v>-</v>
-      </c>
-      <c r="L54" s="206" t="str">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="L54" s="164" t="str">
         <f>IF($F$54=1,"Please explain how methods and tools will be openly available to the public",IF($F$54=2,"Please explain why the sharing of methods and/or tools is unknown?",IF($F$54=3,"This selection has passed a tolerance. Please explain why methods and/or will not be openly available to the public",IF($J$54=1,"Please explain the omission of this item","Please select an option in cell D54"))))</f>
-        <v>Please select an option in cell D54</v>
-      </c>
-      <c r="M54" s="207"/>
-      <c r="N54" s="229"/>
-      <c r="O54" s="230"/>
+        <v>Please explain why the sharing of methods and/or tools is unknown?</v>
+      </c>
+      <c r="M54" s="165"/>
+      <c r="N54" s="154" t="s">
+        <v>177</v>
+      </c>
+      <c r="O54" s="155"/>
       <c r="P54" s="16">
         <f>IF(SUM(I54)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="2:16" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B55" s="55">
+      <c r="B55" s="53">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C55" s="126" t="s">
+      <c r="C55" s="124" t="s">
         <v>78</v>
       </c>
-      <c r="D55" s="157"/>
-      <c r="E55" s="158"/>
-      <c r="F55" s="38" t="str">
+      <c r="D55" s="172" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" s="173"/>
+      <c r="F55" s="36">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G55:$I55,-1)), "")</f>
-        <v/>
-      </c>
-      <c r="G55" s="103" t="str">
+        <v>1</v>
+      </c>
+      <c r="G55" s="101">
         <f>IF($D$55="Data will be curated based on data retention policies and it will be available for re-use by the wider research community",1,"")</f>
-        <v/>
-      </c>
-      <c r="H55" s="104" t="str">
+        <v>1</v>
+      </c>
+      <c r="H55" s="102" t="str">
         <f>IF($D$55="It is unsure whether data will be available for re-use, and/or data retention policies are not known/unclear",1,"")</f>
         <v/>
       </c>
-      <c r="I55" s="105" t="str">
+      <c r="I55" s="103" t="str">
         <f>IF($D$55="Data will not be available for re-use, or data retention policies are not in place",1,"")</f>
         <v/>
       </c>
-      <c r="J55" s="96" t="str">
+      <c r="J55" s="94" t="str">
         <f>IF($D$55="N/A: Omit this item when data sharing agreements or original consent does not allow re-use of the dataset.",1,"")</f>
         <v/>
       </c>
-      <c r="K55" s="33" t="str">
+      <c r="K55" s="31">
         <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
-      <c r="L55" s="200" t="str">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="L55" s="183" t="str">
         <f>IF($F$55=1,"Please state the data retention policy for this project, and explain how the data will be available for re-use",IF($F$55=2,"Please explain why the re-use of data is unknown, and/or why are data retention polcies unclear?",IF($F$55=3,"This selection has passed a tolerance. Please explain why data will not be availabe for re-use, or why data retention policies are not in place",IF($J$55=1,"Please explain why the dataset(s) cannot be re-used","Please select an option in cell D55"))))</f>
-        <v>Please select an option in cell D55</v>
-      </c>
-      <c r="M55" s="201"/>
-      <c r="N55" s="231"/>
-      <c r="O55" s="232"/>
+        <v>Please state the data retention policy for this project, and explain how the data will be available for re-use</v>
+      </c>
+      <c r="M55" s="184"/>
+      <c r="N55" s="156" t="s">
+        <v>176</v>
+      </c>
+      <c r="O55" s="157"/>
       <c r="P55" s="16">
         <f>IF(SUM(I55)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:16" ht="54" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="L56" s="61"/>
-      <c r="M56" s="61"/>
+      <c r="L56" s="59"/>
+      <c r="M56" s="59"/>
       <c r="P56" s="22"/>
     </row>
     <row r="57" spans="2:16" ht="47.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="N57" s="216" t="s">
+      <c r="N57" s="137" t="s">
         <v>150</v>
       </c>
-      <c r="O57" s="216"/>
+      <c r="O57" s="137"/>
     </row>
     <row r="66" spans="16:16" hidden="1" x14ac:dyDescent="0.5">
-      <c r="P66" s="139"/>
+      <c r="P66" s="220"/>
     </row>
     <row r="67" spans="16:16" hidden="1" x14ac:dyDescent="0.5">
-      <c r="P67" s="139"/>
+      <c r="P67" s="220"/>
     </row>
     <row r="68" spans="16:16" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="P68" s="139"/>
+      <c r="P68" s="220"/>
     </row>
     <row r="69" spans="16:16" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="P69" s="139"/>
+      <c r="P69" s="220"/>
     </row>
     <row r="70" spans="16:16" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="P70" s="139"/>
+      <c r="P70" s="220"/>
     </row>
     <row r="71" spans="16:16" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="P71" s="139"/>
+      <c r="P71" s="220"/>
     </row>
     <row r="72" spans="16:16" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="P72" s="139"/>
+      <c r="P72" s="220"/>
     </row>
     <row r="73" spans="16:16" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="P73" s="139"/>
+      <c r="P73" s="220"/>
     </row>
     <row r="74" spans="16:16" hidden="1" x14ac:dyDescent="0.5">
-      <c r="P74" s="139"/>
+      <c r="P74" s="220"/>
     </row>
     <row r="75" spans="16:16" hidden="1" x14ac:dyDescent="0.5">
-      <c r="P75" s="139"/>
+      <c r="P75" s="220"/>
     </row>
     <row r="76" spans="16:16" hidden="1" x14ac:dyDescent="0.5">
-      <c r="P76" s="139"/>
+      <c r="P76" s="220"/>
     </row>
     <row r="77" spans="16:16" hidden="1" x14ac:dyDescent="0.5">
-      <c r="P77" s="139"/>
+      <c r="P77" s="220"/>
     </row>
     <row r="1048576" spans="15:15" hidden="1" x14ac:dyDescent="0.5">
-      <c r="O1048576" s="61"/>
+      <c r="O1048576" s="59"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BQmOtmUROdBToi7l77hhhud6Bo0c/G4ZFtWzh7lYkH91HMJj1Z280byvkwYlS2ZyOGJEpIQYeLG0ZD1SnN9gwA==" saltValue="N19zbME1rV6I1G6Ha2uGcg==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatRows="0" selectLockedCells="1"/>
   <mergeCells count="112">
+    <mergeCell ref="P66:P77"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="L21:L24"/>
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="C7:L7"/>
+    <mergeCell ref="C10:L10"/>
+    <mergeCell ref="C13:L13"/>
+    <mergeCell ref="C16:L16"/>
+    <mergeCell ref="C6:L6"/>
+    <mergeCell ref="C9:L9"/>
+    <mergeCell ref="C12:L12"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="L55:M55"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="L50:M50"/>
+    <mergeCell ref="L51:M51"/>
+    <mergeCell ref="L52:M52"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="L54:M54"/>
+    <mergeCell ref="L53:M53"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="N31:O31"/>
     <mergeCell ref="N57:O57"/>
     <mergeCell ref="M21:N24"/>
     <mergeCell ref="L19:N20"/>
@@ -5762,94 +6028,6 @@
     <mergeCell ref="N41:O41"/>
     <mergeCell ref="N32:O32"/>
     <mergeCell ref="N33:O33"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="L55:M55"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="L50:M50"/>
-    <mergeCell ref="L51:M51"/>
-    <mergeCell ref="L52:M52"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="L54:M54"/>
-    <mergeCell ref="L53:M53"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="L21:L24"/>
-    <mergeCell ref="C4:L4"/>
-    <mergeCell ref="C7:L7"/>
-    <mergeCell ref="C10:L10"/>
-    <mergeCell ref="C13:L13"/>
-    <mergeCell ref="C16:L16"/>
-    <mergeCell ref="C6:L6"/>
-    <mergeCell ref="C9:L9"/>
-    <mergeCell ref="C12:L12"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="P66:P77"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D43:E43"/>
   </mergeCells>
   <conditionalFormatting sqref="B19:D19 H19">
     <cfRule type="containsText" dxfId="45" priority="38" operator="containsText" text="Have you considered these questions?">
@@ -6173,18 +6351,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Retention xmlns="6dab36e7-c487-4780-8e35-3b48fa83d7a8">0</Retention>
-    <EDRMSOwner xmlns="6dab36e7-c487-4780-8e35-3b48fa83d7a8" xsi:nil="true"/>
-    <Record_Type xmlns="6dab36e7-c487-4780-8e35-3b48fa83d7a8">Correspondence, Guidance etc</Record_Type>
-    <RetentionDate xmlns="6dab36e7-c487-4780-8e35-3b48fa83d7a8" xsi:nil="true"/>
-    <RetentionType xmlns="6dab36e7-c487-4780-8e35-3b48fa83d7a8">Notify</RetentionType>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009DF35214976B1543B35A152A7641D3E7" ma:contentTypeVersion="34" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c58e4fea69d58fa215b1b5a0e4da38e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dab36e7-c487-4780-8e35-3b48fa83d7a8" xmlns:ns3="98736429-eed7-4eeb-89bc-06743e71e413" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="abee5eb69777f2c94156cd4ea47bad49" ns2:_="" ns3:_="">
     <xsd:import namespace="6dab36e7-c487-4780-8e35-3b48fa83d7a8"/>
@@ -6456,22 +6622,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Retention xmlns="6dab36e7-c487-4780-8e35-3b48fa83d7a8">0</Retention>
+    <EDRMSOwner xmlns="6dab36e7-c487-4780-8e35-3b48fa83d7a8" xsi:nil="true"/>
+    <Record_Type xmlns="6dab36e7-c487-4780-8e35-3b48fa83d7a8">Correspondence, Guidance etc</Record_Type>
+    <RetentionDate xmlns="6dab36e7-c487-4780-8e35-3b48fa83d7a8" xsi:nil="true"/>
+    <RetentionType xmlns="6dab36e7-c487-4780-8e35-3b48fa83d7a8">Notify</RetentionType>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{682AC2EE-0B14-436F-A00B-D74F0C6291E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6dab36e7-c487-4780-8e35-3b48fa83d7a8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF4DF176-F09A-44AA-B9C6-B14A82562611}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6490,6 +6658,16 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{682AC2EE-0B14-436F-A00B-D74F0C6291E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6dab36e7-c487-4780-8e35-3b48fa83d7a8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BA0B1F6-4CF4-4794-A965-695655EABB38}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Again language correction and style modification
</commit_message>
<xml_diff>
--- a/final_documents/Self-Assessment_Data Ethics.xlsx
+++ b/final_documents/Self-Assessment_Data Ethics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\AI4Good\AI4Good\final_documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jschu\AI4Good\final_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44042EB3-DE23-4886-ACFB-019752E9C73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4095D6-90E5-4348-ADF8-F87EDE1746EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="12800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessment" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,21 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Assessment!$A$1:$P$56</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -616,12 +629,6 @@
     <t>Start date: 04.03.25 (Kick Off Climate), key dates: 24.03.25 (Meeting with Basil and project explanation), 25.03.25 (Milestone I), 15.04.25 (Milestone II), 12.05.25 (Milestone III), 24.05.25 (Final submission), end date: 26.05.25 (Presentation)</t>
   </si>
   <si>
-    <t>Interactive dashboard of runoff data and model sensitivity. Project partnes:  Gudmundsson Lukas and Kraft Basil, no sponsors.</t>
-  </si>
-  <si>
-    <t>How data are collected: Project data were provided by Kraft Basil. How was data used: Integration in interactive dashboard, ai training and calculation of model sensitivity. Research environment used: Python with VS Code and Pycharm.</t>
-  </si>
-  <si>
     <t>https://www.research-collection.ethz.ch/handle/20.500.11850/714281, CH-RUN: Runoff reconstruction for Switzerland (CHRUN_v1)</t>
   </si>
   <si>
@@ -637,24 +644,12 @@
     <t>No.</t>
   </si>
   <si>
-    <t>Primary goal was visualisation of data and as supplement we implemented a sensitvity model.</t>
-  </si>
-  <si>
     <t>Societal benefits might be limited to certain groups/areas</t>
   </si>
   <si>
-    <t>Groups that work with water runoff data in Switzerland.</t>
-  </si>
-  <si>
-    <t>No personal data used in the project. Probably wrong AI predictions could lead to wrong assumptions, if model predicts wrong sensitivity values.</t>
-  </si>
-  <si>
     <t>The data was processed to the best of our knowledge and belief.</t>
   </si>
   <si>
-    <t>Data doesn't contains personal data.</t>
-  </si>
-  <si>
     <t>Basic data security measures are in place (e.g. institutional storage ETH, version control), and no further special arrangements are currently required.</t>
   </si>
   <si>
@@ -682,16 +677,36 @@
     <t>Public views are at this moment unknown.</t>
   </si>
   <si>
-    <t>Public engagement was not part of the project goal.</t>
-  </si>
-  <si>
     <t>Stored in gitlab repository.</t>
   </si>
   <si>
     <t>The sharing of methods and tools has not yet been confirmed.</t>
   </si>
   <si>
-    <t>Public access to research outcomes is currently uncertain.</t>
+    <t>The primary goal was the visualization of data. Additionally, we implemented a sensitivity model to supplement the analysis.”</t>
+  </si>
+  <si>
+    <t>The societal benefit is primarily targeted at groups working with water runoff data in Switzerland.</t>
+  </si>
+  <si>
+    <t>No personal data was used in the project. However, inaccurate AI predictions could potentially lead to incorrect assumptions if the model poorly estimates sensitivity values.</t>
+  </si>
+  <si>
+    <t>The data doesn't contain personal data.</t>
+  </si>
+  <si>
+    <t>Public engagement was not an objective of the project and was therefore not conducted.</t>
+  </si>
+  <si>
+    <t>It is currently unclear whether research outcomes will be made publicly accessible.</t>
+  </si>
+  <si>
+    <t>Interactive dashboard of runoff data and model sensitivity. Project partners: Lukas Gudmundsson and Basil Kraft. No sponsors.</t>
+  </si>
+  <si>
+    <t>How data are collected: Project data were provided by Basil Kraft.
+How data are used: Integrated into an interactive dashboard; used for AI model training and sensitivity analysis.
+Research environment: Python, using VS Code and PyCharm.</t>
   </si>
 </sst>
 </file>
@@ -2458,63 +2473,294 @@
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="15" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="1" fontId="15" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
@@ -2526,6 +2772,74 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -2542,14 +2856,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="53" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -2564,297 +2870,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -3664,38 +3679,38 @@
   </sheetPr>
   <dimension ref="A1:XFC1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1048576" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N54" sqref="N54:O54"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="86" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.35" zeroHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.87890625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.41015625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="24" style="1" customWidth="1"/>
-    <col min="5" max="5" width="57.29296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.41015625" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1171875" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1171875" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5859375" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="57.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" style="1" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="17.87890625" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="31.5859375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="24.29296875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="26.1171875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="41.5859375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="3.5859375" style="17" customWidth="1"/>
-    <col min="17" max="17" width="20.5859375" style="17" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5859375" style="17" hidden="1" customWidth="1"/>
-    <col min="19" max="16380" width="8.87890625" style="17" hidden="1"/>
-    <col min="16381" max="16381" width="27.87890625" style="17" hidden="1" customWidth="1"/>
-    <col min="16382" max="16382" width="51.29296875" style="17" hidden="1" customWidth="1"/>
-    <col min="16383" max="16383" width="20.5859375" style="17" hidden="1" customWidth="1"/>
-    <col min="16384" max="16384" width="6.41015625" style="17" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="31.5546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="24.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="26.109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="41.5546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="3.5546875" style="17" customWidth="1"/>
+    <col min="17" max="17" width="20.5546875" style="17" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5546875" style="17" hidden="1" customWidth="1"/>
+    <col min="19" max="16380" width="8.88671875" style="17" hidden="1"/>
+    <col min="16381" max="16381" width="27.88671875" style="17" hidden="1" customWidth="1"/>
+    <col min="16382" max="16382" width="51.33203125" style="17" hidden="1" customWidth="1"/>
+    <col min="16383" max="16383" width="20.5546875" style="17" hidden="1" customWidth="1"/>
+    <col min="16384" max="16384" width="6.44140625" style="17" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16 16381:16383" s="4" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:16 16381:16383" s="4" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -3717,7 +3732,7 @@
       <c r="O1" s="40"/>
       <c r="P1" s="3"/>
     </row>
-    <row r="2" spans="1:16 16381:16383" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:16 16381:16383" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -3735,7 +3750,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="7"/>
     </row>
-    <row r="3" spans="1:16 16381:16383" s="4" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:16 16381:16383" s="4" customFormat="1" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -3753,23 +3768,23 @@
       <c r="O3" s="8"/>
       <c r="P3" s="7"/>
     </row>
-    <row r="4" spans="1:16 16381:16383" s="4" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:16 16381:16383" s="4" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="204" t="s">
+      <c r="C4" s="177" t="s">
         <v>151</v>
       </c>
-      <c r="D4" s="205"/>
-      <c r="E4" s="205"/>
-      <c r="F4" s="205"/>
-      <c r="G4" s="205"/>
-      <c r="H4" s="205"/>
-      <c r="I4" s="205"/>
-      <c r="J4" s="205"/>
-      <c r="K4" s="205"/>
-      <c r="L4" s="206"/>
+      <c r="D4" s="178"/>
+      <c r="E4" s="178"/>
+      <c r="F4" s="178"/>
+      <c r="G4" s="178"/>
+      <c r="H4" s="178"/>
+      <c r="I4" s="178"/>
+      <c r="J4" s="178"/>
+      <c r="K4" s="178"/>
+      <c r="L4" s="179"/>
       <c r="M4" s="45"/>
       <c r="N4" s="45"/>
       <c r="O4" s="45"/>
@@ -3784,7 +3799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:16 16381:16383" s="4" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:16 16381:16383" s="4" customFormat="1" ht="6.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -3805,23 +3820,23 @@
       <c r="XFB5" s="75"/>
       <c r="XFC5" s="75"/>
     </row>
-    <row r="6" spans="1:16 16381:16383" s="4" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:16 16381:16383" s="4" customFormat="1" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
-      <c r="B6" s="217" t="s">
+      <c r="B6" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="213" t="s">
+      <c r="C6" s="186" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="213"/>
-      <c r="E6" s="213"/>
-      <c r="F6" s="213"/>
-      <c r="G6" s="213"/>
-      <c r="H6" s="213"/>
-      <c r="I6" s="213"/>
-      <c r="J6" s="213"/>
-      <c r="K6" s="213"/>
-      <c r="L6" s="213"/>
+      <c r="D6" s="186"/>
+      <c r="E6" s="186"/>
+      <c r="F6" s="186"/>
+      <c r="G6" s="186"/>
+      <c r="H6" s="186"/>
+      <c r="I6" s="186"/>
+      <c r="J6" s="186"/>
+      <c r="K6" s="186"/>
+      <c r="L6" s="186"/>
       <c r="M6" s="45"/>
       <c r="N6" s="45"/>
       <c r="O6" s="45"/>
@@ -3836,21 +3851,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:16 16381:16383" s="4" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:16 16381:16383" s="4" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
-      <c r="B7" s="217"/>
-      <c r="C7" s="204" t="s">
+      <c r="B7" s="190"/>
+      <c r="C7" s="177" t="s">
         <v>152</v>
       </c>
-      <c r="D7" s="205"/>
-      <c r="E7" s="205"/>
-      <c r="F7" s="205"/>
-      <c r="G7" s="205"/>
-      <c r="H7" s="205"/>
-      <c r="I7" s="205"/>
-      <c r="J7" s="205"/>
-      <c r="K7" s="205"/>
-      <c r="L7" s="206"/>
+      <c r="D7" s="178"/>
+      <c r="E7" s="178"/>
+      <c r="F7" s="178"/>
+      <c r="G7" s="178"/>
+      <c r="H7" s="178"/>
+      <c r="I7" s="178"/>
+      <c r="J7" s="178"/>
+      <c r="K7" s="178"/>
+      <c r="L7" s="179"/>
       <c r="M7" s="45"/>
       <c r="N7" s="45"/>
       <c r="O7" s="45"/>
@@ -3865,19 +3880,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:16 16381:16383" s="4" customFormat="1" ht="8.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:16 16381:16383" s="4" customFormat="1" ht="8.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="219"/>
-      <c r="D8" s="219"/>
-      <c r="E8" s="219"/>
-      <c r="F8" s="219"/>
-      <c r="G8" s="219"/>
-      <c r="H8" s="219"/>
-      <c r="I8" s="219"/>
-      <c r="J8" s="219"/>
-      <c r="K8" s="219"/>
-      <c r="L8" s="219"/>
+      <c r="C8" s="192"/>
+      <c r="D8" s="192"/>
+      <c r="E8" s="192"/>
+      <c r="F8" s="192"/>
+      <c r="G8" s="192"/>
+      <c r="H8" s="192"/>
+      <c r="I8" s="192"/>
+      <c r="J8" s="192"/>
+      <c r="K8" s="192"/>
+      <c r="L8" s="192"/>
       <c r="M8" s="45"/>
       <c r="N8" s="45"/>
       <c r="O8" s="45"/>
@@ -3892,23 +3907,23 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:16 16381:16383" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:16 16381:16383" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
-      <c r="B9" s="218" t="s">
+      <c r="B9" s="191" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="214" t="s">
+      <c r="C9" s="187" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="214"/>
-      <c r="E9" s="214"/>
-      <c r="F9" s="214"/>
-      <c r="G9" s="214"/>
-      <c r="H9" s="214"/>
-      <c r="I9" s="214"/>
-      <c r="J9" s="214"/>
-      <c r="K9" s="214"/>
-      <c r="L9" s="214"/>
+      <c r="D9" s="187"/>
+      <c r="E9" s="187"/>
+      <c r="F9" s="187"/>
+      <c r="G9" s="187"/>
+      <c r="H9" s="187"/>
+      <c r="I9" s="187"/>
+      <c r="J9" s="187"/>
+      <c r="K9" s="187"/>
+      <c r="L9" s="187"/>
       <c r="M9" s="45"/>
       <c r="N9" s="45"/>
       <c r="O9" s="45"/>
@@ -3923,21 +3938,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:16 16381:16383" s="4" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:16 16381:16383" s="4" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="218"/>
-      <c r="C10" s="204" t="s">
-        <v>153</v>
-      </c>
-      <c r="D10" s="205"/>
-      <c r="E10" s="205"/>
-      <c r="F10" s="205"/>
-      <c r="G10" s="205"/>
-      <c r="H10" s="205"/>
-      <c r="I10" s="205"/>
-      <c r="J10" s="205"/>
-      <c r="K10" s="205"/>
-      <c r="L10" s="206"/>
+      <c r="B10" s="191"/>
+      <c r="C10" s="177" t="s">
+        <v>177</v>
+      </c>
+      <c r="D10" s="178"/>
+      <c r="E10" s="178"/>
+      <c r="F10" s="178"/>
+      <c r="G10" s="178"/>
+      <c r="H10" s="178"/>
+      <c r="I10" s="178"/>
+      <c r="J10" s="178"/>
+      <c r="K10" s="178"/>
+      <c r="L10" s="179"/>
       <c r="M10" s="45"/>
       <c r="N10" s="130" t="s">
         <v>22</v>
@@ -3954,7 +3969,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:16 16381:16383" s="4" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:16 16381:16383" s="4" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -3980,23 +3995,23 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:16 16381:16383" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:16 16381:16383" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
-      <c r="B12" s="218" t="s">
+      <c r="B12" s="191" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="215" t="s">
+      <c r="C12" s="188" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="215"/>
-      <c r="E12" s="215"/>
-      <c r="F12" s="215"/>
-      <c r="G12" s="215"/>
-      <c r="H12" s="215"/>
-      <c r="I12" s="215"/>
-      <c r="J12" s="215"/>
-      <c r="K12" s="215"/>
-      <c r="L12" s="215"/>
+      <c r="D12" s="188"/>
+      <c r="E12" s="188"/>
+      <c r="F12" s="188"/>
+      <c r="G12" s="188"/>
+      <c r="H12" s="188"/>
+      <c r="I12" s="188"/>
+      <c r="J12" s="188"/>
+      <c r="K12" s="188"/>
+      <c r="L12" s="188"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
@@ -4011,21 +4026,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:16 16381:16383" s="4" customFormat="1" ht="205.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:16 16381:16383" s="4" customFormat="1" ht="205.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="218"/>
-      <c r="C13" s="207" t="s">
-        <v>154</v>
-      </c>
-      <c r="D13" s="208"/>
-      <c r="E13" s="208"/>
-      <c r="F13" s="208"/>
-      <c r="G13" s="208"/>
-      <c r="H13" s="208"/>
-      <c r="I13" s="208"/>
-      <c r="J13" s="208"/>
-      <c r="K13" s="208"/>
-      <c r="L13" s="209"/>
+      <c r="B13" s="191"/>
+      <c r="C13" s="180" t="s">
+        <v>178</v>
+      </c>
+      <c r="D13" s="181"/>
+      <c r="E13" s="181"/>
+      <c r="F13" s="181"/>
+      <c r="G13" s="181"/>
+      <c r="H13" s="181"/>
+      <c r="I13" s="181"/>
+      <c r="J13" s="181"/>
+      <c r="K13" s="181"/>
+      <c r="L13" s="182"/>
       <c r="N13" s="65"/>
       <c r="O13" s="65"/>
       <c r="P13" s="11"/>
@@ -4039,7 +4054,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:16 16381:16383" s="4" customFormat="1" ht="3.95" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:16 16381:16383" s="4" customFormat="1" ht="3.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="8"/>
       <c r="C14" s="7"/>
@@ -4066,23 +4081,23 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:16 16381:16383" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:16 16381:16383" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
-      <c r="B15" s="218" t="s">
+      <c r="B15" s="191" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="216" t="s">
+      <c r="C15" s="189" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="216"/>
-      <c r="E15" s="216"/>
-      <c r="F15" s="216"/>
-      <c r="G15" s="216"/>
-      <c r="H15" s="216"/>
-      <c r="I15" s="216"/>
-      <c r="J15" s="216"/>
-      <c r="K15" s="216"/>
-      <c r="L15" s="216"/>
+      <c r="D15" s="189"/>
+      <c r="E15" s="189"/>
+      <c r="F15" s="189"/>
+      <c r="G15" s="189"/>
+      <c r="H15" s="189"/>
+      <c r="I15" s="189"/>
+      <c r="J15" s="189"/>
+      <c r="K15" s="189"/>
+      <c r="L15" s="189"/>
       <c r="M15" s="38"/>
       <c r="N15" s="38"/>
       <c r="O15" s="38"/>
@@ -4097,21 +4112,21 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:16 16381:16383" s="4" customFormat="1" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:16 16381:16383" s="4" customFormat="1" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
-      <c r="B16" s="218"/>
-      <c r="C16" s="210" t="s">
-        <v>155</v>
-      </c>
-      <c r="D16" s="211"/>
-      <c r="E16" s="211"/>
-      <c r="F16" s="211"/>
-      <c r="G16" s="211"/>
-      <c r="H16" s="211"/>
-      <c r="I16" s="211"/>
-      <c r="J16" s="211"/>
-      <c r="K16" s="211"/>
-      <c r="L16" s="212"/>
+      <c r="B16" s="191"/>
+      <c r="C16" s="183" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" s="184"/>
+      <c r="E16" s="184"/>
+      <c r="F16" s="184"/>
+      <c r="G16" s="184"/>
+      <c r="H16" s="184"/>
+      <c r="I16" s="184"/>
+      <c r="J16" s="184"/>
+      <c r="K16" s="184"/>
+      <c r="L16" s="185"/>
       <c r="M16" s="39"/>
       <c r="N16" s="39"/>
       <c r="O16" s="39"/>
@@ -4126,7 +4141,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:18 16381:16383" s="4" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:18 16381:16383" s="4" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -4153,7 +4168,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:18 16381:16383" s="4" customFormat="1" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:18 16381:16383" s="4" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="46"/>
       <c r="C18" s="46"/>
@@ -4180,13 +4195,13 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:18 16381:16383" s="4" customFormat="1" ht="58.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:18 16381:16383" s="4" customFormat="1" ht="58.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
-      <c r="B19" s="197" t="str">
+      <c r="B19" s="170" t="str">
         <f>IF(SUM(I20:I24)=0,"Have you considered these questions?","")</f>
         <v/>
       </c>
-      <c r="C19" s="198"/>
+      <c r="C19" s="171"/>
       <c r="D19" s="13" t="s">
         <v>54</v>
       </c>
@@ -4200,11 +4215,11 @@
       </c>
       <c r="J19" s="64"/>
       <c r="K19" s="69"/>
-      <c r="L19" s="144" t="s">
+      <c r="L19" s="223" t="s">
         <v>57</v>
       </c>
-      <c r="M19" s="145"/>
-      <c r="N19" s="146"/>
+      <c r="M19" s="224"/>
+      <c r="N19" s="225"/>
       <c r="O19" s="60"/>
       <c r="P19" s="11"/>
       <c r="XFA19" s="76" t="s">
@@ -4217,14 +4232,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:18 16381:16383" s="4" customFormat="1" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:18 16381:16383" s="4" customFormat="1" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
-      <c r="B20" s="189" t="s">
+      <c r="B20" s="162" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="190"/>
-      <c r="D20" s="235" t="s">
-        <v>157</v>
+      <c r="C20" s="163"/>
+      <c r="D20" s="137" t="s">
+        <v>155</v>
       </c>
       <c r="E20" s="134" t="s">
         <v>62</v>
@@ -4240,9 +4255,9 @@
       </c>
       <c r="J20" s="64"/>
       <c r="K20" s="69"/>
-      <c r="L20" s="147"/>
-      <c r="M20" s="148"/>
-      <c r="N20" s="149"/>
+      <c r="L20" s="226"/>
+      <c r="M20" s="227"/>
+      <c r="N20" s="228"/>
       <c r="O20" s="60"/>
       <c r="R20" s="132" t="s">
         <v>63</v>
@@ -4257,14 +4272,14 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:18 16381:16383" s="4" customFormat="1" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:18 16381:16383" s="4" customFormat="1" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
-      <c r="B21" s="191" t="s">
+      <c r="B21" s="164" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="192"/>
-      <c r="D21" s="236" t="s">
-        <v>156</v>
+      <c r="C21" s="165"/>
+      <c r="D21" s="138" t="s">
+        <v>154</v>
       </c>
       <c r="E21" s="113">
         <f>IF(COUNTBLANK($N$28:$N$55)&gt;0,1,0)</f>
@@ -4281,15 +4296,15 @@
       </c>
       <c r="J21" s="70"/>
       <c r="K21" s="69"/>
-      <c r="L21" s="201" t="str">
+      <c r="L21" s="174" t="str">
         <f>IF(AND($E$21=1,$E$24&gt;=1),"-",IF($E$24&gt;=1,"-",IF($E$21=1,"-",IF($R$21&lt;1,"Green",IF(AND($R$21&gt;=1,$R$21&lt;1.6),"Green",IF(AND($R$21&gt;=1.6,$R$21&lt;2.3),"Amber",IF(AND($R$21&gt;=2.3,$R$21&lt;3),"Red",IF(AND($R$21&gt;=3,$R$21&lt;=100),"Red","-"))))))))</f>
         <v>Amber</v>
       </c>
-      <c r="M21" s="138" t="str">
+      <c r="M21" s="217" t="str">
         <f>IF(AND($E$21=1,$E$24&gt;=1),"Form not complete, please select an option in each of the drop down boxes and provide justifications",IF($E$24&gt;=1,"Form not complete, please select an option in each of the drop down boxes",IF($E$21=1,"One or more justifications have been left blank, please complete all justifications as per the justification suggestion",IF(SUM(P27:P55)&gt;0,"One or more items have reached or exceeded a tolerance level - consult with the Data Ethics team",IF($R$21&lt;1,"Very low risk - project may proceed after confirmation from the Data Ethics team",IF(AND($R$21&gt;=1,$R$21&lt;1.6),"Low risk - project may proceed after confirmation from the Data Ethics team",IF(AND($R$21&gt;=1.6,$R$21&lt;2.3),"Average risk - consult with the Data Ethics team to discuss actions to mitigate any highlighted risks before proceeding with the project",IF(AND($R$21&gt;=2.3,$R$21&lt;3),"High risk - consult with the Data Ethics team. If risks cannot be mitigated then this project should be presented to NSDEC for a full independent ethical review before proceeding",IF(AND($R$21&gt;=3,$R$21&lt;=100),"Very High risk - consult with the Data Ethics team. If risks cannot be mitigated then this project should be presented to NSDEC for a full independent ethical review before proceeding","Project requires an ethical review before proceeding, please select an option in each of the drop down boxes")))))))))</f>
         <v>One or more items have reached or exceeded a tolerance level - consult with the Data Ethics team</v>
       </c>
-      <c r="N21" s="139"/>
+      <c r="N21" s="218"/>
       <c r="O21" s="126"/>
       <c r="R21" s="133">
         <f>IFERROR(AVERAGE(K30,K36,K42,K47,K50,K53)*PRODUCT($H$20:$H$23),"-")</f>
@@ -4305,14 +4320,14 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:18 16381:16383" s="4" customFormat="1" ht="48.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:18 16381:16383" s="4" customFormat="1" ht="48.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
-      <c r="B22" s="193" t="s">
+      <c r="B22" s="166" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="194"/>
-      <c r="D22" s="236" t="s">
-        <v>158</v>
+      <c r="C22" s="167"/>
+      <c r="D22" s="138" t="s">
+        <v>156</v>
       </c>
       <c r="E22" s="113">
         <f>IF(COUNTBLANK($D$30:$D$55)&gt;0,1,0)</f>
@@ -4329,9 +4344,9 @@
       </c>
       <c r="J22" s="64"/>
       <c r="K22" s="69"/>
-      <c r="L22" s="202"/>
-      <c r="M22" s="140"/>
-      <c r="N22" s="141"/>
+      <c r="L22" s="175"/>
+      <c r="M22" s="219"/>
+      <c r="N22" s="220"/>
       <c r="O22" s="61"/>
       <c r="XFA22" s="74" t="s">
         <v>72</v>
@@ -4343,14 +4358,14 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:18 16381:16383" s="4" customFormat="1" ht="101.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:18 16381:16383" s="4" customFormat="1" ht="101.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
-      <c r="B23" s="195" t="s">
+      <c r="B23" s="168" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="196"/>
+      <c r="C23" s="169"/>
       <c r="D23" s="41" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E23" s="113">
         <f>IF(COUNTBLANK($E$29)&gt;0,1,0)</f>
@@ -4367,9 +4382,9 @@
       </c>
       <c r="J23" s="64"/>
       <c r="K23" s="69"/>
-      <c r="L23" s="202"/>
-      <c r="M23" s="140"/>
-      <c r="N23" s="141"/>
+      <c r="L23" s="175"/>
+      <c r="M23" s="219"/>
+      <c r="N23" s="220"/>
       <c r="O23" s="61"/>
       <c r="XFA23" s="76" t="s">
         <v>76</v>
@@ -4381,10 +4396,10 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:18 16381:16383" s="4" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:18 16381:16383" s="4" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
-      <c r="B24" s="221"/>
-      <c r="C24" s="222"/>
+      <c r="B24" s="140"/>
+      <c r="C24" s="141"/>
       <c r="D24" s="117"/>
       <c r="E24" s="135">
         <f>SUM($E$22,$E$23)</f>
@@ -4395,9 +4410,9 @@
       <c r="I24" s="64"/>
       <c r="J24" s="64"/>
       <c r="K24" s="69"/>
-      <c r="L24" s="203"/>
-      <c r="M24" s="142"/>
-      <c r="N24" s="143"/>
+      <c r="L24" s="176"/>
+      <c r="M24" s="221"/>
+      <c r="N24" s="222"/>
       <c r="O24" s="61"/>
       <c r="XFA24" s="76" t="s">
         <v>79</v>
@@ -4409,7 +4424,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:18 16381:16383" s="4" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:18 16381:16383" s="4" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="43"/>
       <c r="C25" s="43"/>
@@ -4433,7 +4448,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:18 16381:16383" s="4" customFormat="1" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:18 16381:16383" s="4" customFormat="1" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -4460,33 +4475,33 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:18 16381:16383" ht="127.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:18 16381:16383" ht="127.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="56"/>
       <c r="C27" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="199" t="s">
+      <c r="D27" s="172" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="200"/>
+      <c r="E27" s="173"/>
       <c r="F27" s="15"/>
-      <c r="G27" s="231" t="s">
+      <c r="G27" s="154" t="s">
         <v>90</v>
       </c>
-      <c r="H27" s="232"/>
-      <c r="I27" s="232"/>
-      <c r="J27" s="233"/>
+      <c r="H27" s="155"/>
+      <c r="I27" s="155"/>
+      <c r="J27" s="156"/>
       <c r="K27" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="L27" s="181" t="s">
+      <c r="L27" s="198" t="s">
         <v>92</v>
       </c>
-      <c r="M27" s="182"/>
-      <c r="N27" s="166" t="s">
+      <c r="M27" s="199"/>
+      <c r="N27" s="208" t="s">
         <v>93</v>
       </c>
-      <c r="O27" s="167"/>
+      <c r="O27" s="209"/>
       <c r="P27" s="16"/>
       <c r="XFA27" s="81" t="s">
         <v>94</v>
@@ -4498,7 +4513,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:18 16381:16383" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:18 16381:16383" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="78"/>
       <c r="B28" s="112" t="s">
         <v>97</v>
@@ -4506,10 +4521,10 @@
       <c r="C28" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="176" t="s">
+      <c r="D28" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="E28" s="175"/>
+      <c r="E28" s="160"/>
       <c r="F28" s="35" t="s">
         <v>100</v>
       </c>
@@ -4529,14 +4544,14 @@
         <f>K31</f>
         <v>1.5</v>
       </c>
-      <c r="L28" s="150" t="s">
+      <c r="L28" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="M28" s="151"/>
-      <c r="N28" s="150" t="s">
+      <c r="M28" s="153"/>
+      <c r="N28" s="152" t="s">
         <v>103</v>
       </c>
-      <c r="O28" s="151"/>
+      <c r="O28" s="153"/>
       <c r="XFA28" s="82" t="s">
         <v>104</v>
       </c>
@@ -4544,7 +4559,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:18 16381:16383" s="48" customFormat="1" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:18 16381:16383" s="48" customFormat="1" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="49">
         <v>1</v>
@@ -4579,15 +4594,15 @@
         <f>K30</f>
         <v>1.5</v>
       </c>
-      <c r="L29" s="164" t="str">
+      <c r="L29" s="206" t="str">
         <f>IF($F$29=1,"Please explain the public good for this project. A link to our public good guidance can be found to the left of the drop down statement",IF($F$29=2,"This selection has passed a tolerance. Please explain the potential public good, and what is to be done to further explore this potential",IF($F$29=3,"This selection has passed a tolerance. Please explain why there is not a public good","Please select an option in cell D29")))</f>
         <v>This selection has passed a tolerance. Please explain the potential public good, and what is to be done to further explore this potential</v>
       </c>
-      <c r="M29" s="165"/>
-      <c r="N29" s="152" t="s">
-        <v>160</v>
-      </c>
-      <c r="O29" s="153"/>
+      <c r="M29" s="207"/>
+      <c r="N29" s="210" t="s">
+        <v>171</v>
+      </c>
+      <c r="O29" s="211"/>
       <c r="P29" s="16">
         <f>IF(SUM(H29:I29)&gt;0, 1, 0)</f>
         <v>1</v>
@@ -4599,7 +4614,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:18 16381:16383" s="48" customFormat="1" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:18 16381:16383" s="48" customFormat="1" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="50">
         <f>IF(IFERROR(SEARCH("Principle", C30, 1)&gt; 1, -1)=-1, B29+1, B29)</f>
@@ -4608,10 +4623,10 @@
       <c r="C30" s="118" t="s">
         <v>110</v>
       </c>
-      <c r="D30" s="177" t="s">
-        <v>161</v>
-      </c>
-      <c r="E30" s="178"/>
+      <c r="D30" s="194" t="s">
+        <v>158</v>
+      </c>
+      <c r="E30" s="195"/>
       <c r="F30" s="33">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G30:$I30,-1)), "")</f>
         <v>2</v>
@@ -4636,15 +4651,15 @@
         <f>IFERROR(AVERAGE(F29:F32),"-")</f>
         <v>1.5</v>
       </c>
-      <c r="L30" s="164" t="str">
+      <c r="L30" s="206" t="str">
         <f>IF($F$30=1,"Please explain how the public good is applicable to the whole population",IF($F$30=2,"Please explain why this is proportional, and provide any mitigations against this limitation",IF($F$30=3,"This selection has passed a tolerance. Please explain why this is limited to certain groups, and provide any mitigations",IF($J$30=1,"Please explain why the research is focused on that specific group, and whether this, or other groups, might be adversely affected by this research","Please select an option in cell D30"))))</f>
         <v>Please explain why this is proportional, and provide any mitigations against this limitation</v>
       </c>
-      <c r="M30" s="165"/>
-      <c r="N30" s="158" t="s">
-        <v>162</v>
-      </c>
-      <c r="O30" s="159"/>
+      <c r="M30" s="207"/>
+      <c r="N30" s="212" t="s">
+        <v>172</v>
+      </c>
+      <c r="O30" s="213"/>
       <c r="P30" s="16">
         <f>IF(SUM(I30:I30)&gt;0, 1, 0)</f>
         <v>0</v>
@@ -4656,7 +4671,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:18 16381:16383" s="48" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:18 16381:16383" s="48" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="50">
         <f t="shared" ref="B31:B55" si="0">IF(IFERROR(SEARCH("Principle", C31, 1)&gt; 1, -1)=-1, B30+1, B30)</f>
@@ -4665,10 +4680,10 @@
       <c r="C31" s="118" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="170" t="s">
+      <c r="D31" s="150" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="171"/>
+      <c r="E31" s="151"/>
       <c r="F31" s="33">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G31:$I31,-1)), "")</f>
         <v>1</v>
@@ -4690,15 +4705,15 @@
         <f>K30</f>
         <v>1.5</v>
       </c>
-      <c r="L31" s="164" t="str">
+      <c r="L31" s="206" t="str">
         <f>IF($F$31=1,"Please explain steps to ensure that there is no potential harm. This includes any potential harm as a result of secondary analysis outcomes",IF($F$31=2,"Please explain why this is proportional, and provide any mitigations against this potential harm",IF($F$31=3,"This selection has passed a tolerance. Please explain this potential harm and why it cannot be mitigated","Please select an option in cell D31")))</f>
         <v>Please explain steps to ensure that there is no potential harm. This includes any potential harm as a result of secondary analysis outcomes</v>
       </c>
-      <c r="M31" s="165"/>
-      <c r="N31" s="168" t="s">
-        <v>163</v>
-      </c>
-      <c r="O31" s="169"/>
+      <c r="M31" s="207"/>
+      <c r="N31" s="214" t="s">
+        <v>173</v>
+      </c>
+      <c r="O31" s="215"/>
       <c r="P31" s="16">
         <f>IF(SUM(I31)&gt;0, 1, 0)</f>
         <v>0</v>
@@ -4710,7 +4725,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="32" spans="1:18 16381:16383" s="48" customFormat="1" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:18 16381:16383" s="48" customFormat="1" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="51">
         <f t="shared" si="0"/>
@@ -4719,10 +4734,10 @@
       <c r="C32" s="119" t="s">
         <v>116</v>
       </c>
-      <c r="D32" s="179" t="s">
+      <c r="D32" s="196" t="s">
         <v>58</v>
       </c>
-      <c r="E32" s="180"/>
+      <c r="E32" s="197"/>
       <c r="F32" s="34">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G32:$I32,-1)), "")</f>
         <v>1</v>
@@ -4744,15 +4759,15 @@
         <f>K30</f>
         <v>1.5</v>
       </c>
-      <c r="L32" s="164" t="str">
+      <c r="L32" s="206" t="str">
         <f>IF($F$32=1,"Please explain steps taken to ensure that there is no bias",IF($F$32=2,"Please explain why this is proportional, and provide any mitigations against this bias",IF($F$32=3,"This selection has passed a tolerance. Please explain this bias and why it cannot be mitigated","Please select an option in cell D32")))</f>
         <v>Please explain steps taken to ensure that there is no bias</v>
       </c>
-      <c r="M32" s="165"/>
-      <c r="N32" s="162" t="s">
-        <v>164</v>
-      </c>
-      <c r="O32" s="163"/>
+      <c r="M32" s="207"/>
+      <c r="N32" s="235" t="s">
+        <v>159</v>
+      </c>
+      <c r="O32" s="236"/>
       <c r="P32" s="16">
         <f>IF(SUM(I32)&gt;0, 1, 0)</f>
         <v>0</v>
@@ -4764,15 +4779,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="2:16 16381:16383" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:16 16381:16383" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="20"/>
       <c r="C33" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="D33" s="234" t="s">
+      <c r="D33" s="159" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="175"/>
+      <c r="E33" s="160"/>
       <c r="F33" s="35" t="s">
         <v>100</v>
       </c>
@@ -4792,14 +4807,14 @@
         <f t="shared" ref="K33:K35" si="1">K34</f>
         <v>1.4</v>
       </c>
-      <c r="L33" s="150" t="s">
+      <c r="L33" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="M33" s="151"/>
-      <c r="N33" s="150" t="s">
+      <c r="M33" s="153"/>
+      <c r="N33" s="152" t="s">
         <v>103</v>
       </c>
-      <c r="O33" s="151"/>
+      <c r="O33" s="153"/>
       <c r="P33" s="16"/>
       <c r="XFA33" s="85" t="s">
         <v>120</v>
@@ -4808,17 +4823,17 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="2:16 16381:16383" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:16 16381:16383" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="49">
         <v>5</v>
       </c>
       <c r="C34" s="120" t="s">
         <v>122</v>
       </c>
-      <c r="D34" s="225" t="s">
+      <c r="D34" s="144" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="226"/>
+      <c r="E34" s="145"/>
       <c r="F34" s="32">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G34:$I34,-1)), "")</f>
         <v>1</v>
@@ -4840,15 +4855,15 @@
         <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
-      <c r="L34" s="164" t="str">
+      <c r="L34" s="206" t="str">
         <f>IF($F$34=1,"Please explain the security arrangments that ensure direct identifcation is not possible",IF($F$34=2,"This selection has passed a tolerance. Please explain what actions will be taken to find out identifiability, and revise this item once known",IF($F$34=3,"This selection has passed a tolerance. Please explain why the data and research outcomes are identifiable and why this cannot be mitigated","Please select an option in cell D34")))</f>
         <v>Please explain the security arrangments that ensure direct identifcation is not possible</v>
       </c>
-      <c r="M34" s="165"/>
-      <c r="N34" s="152" t="s">
-        <v>165</v>
-      </c>
-      <c r="O34" s="153"/>
+      <c r="M34" s="207"/>
+      <c r="N34" s="210" t="s">
+        <v>174</v>
+      </c>
+      <c r="O34" s="211"/>
       <c r="P34" s="16">
         <f>IF(SUM(H34:I34)&gt;0, 1, 0)</f>
         <v>0</v>
@@ -4860,7 +4875,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="50">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4868,10 +4883,10 @@
       <c r="C35" s="118" t="s">
         <v>125</v>
       </c>
-      <c r="D35" s="223" t="s">
+      <c r="D35" s="142" t="s">
         <v>94</v>
       </c>
-      <c r="E35" s="224"/>
+      <c r="E35" s="143"/>
       <c r="F35" s="33">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G35:$I35,-1)), "")</f>
         <v>1</v>
@@ -4893,15 +4908,15 @@
         <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
-      <c r="L35" s="164" t="str">
+      <c r="L35" s="206" t="str">
         <f>IF($F$35=1,"Please explain the security arrangments that ensure indirect identifcation is not possible",IF($F$35=2,"This selection has passed a tolerance. Please explain what actions will be taken to find out identifiability, and revise this item once known",IF($F$35=3,"This selection has passed a tolerance. Please explain why the data and research outcomes are indirectly identifiable and why this cannot be mitigated","Please select an option in cell D35")))</f>
         <v>Please explain the security arrangments that ensure indirect identifcation is not possible</v>
       </c>
-      <c r="M35" s="165"/>
-      <c r="N35" s="158" t="s">
-        <v>165</v>
-      </c>
-      <c r="O35" s="159"/>
+      <c r="M35" s="207"/>
+      <c r="N35" s="212" t="s">
+        <v>174</v>
+      </c>
+      <c r="O35" s="213"/>
       <c r="P35" s="16">
         <f>IF(SUM(H35:I35)&gt;0, 1, 0)</f>
         <v>0</v>
@@ -4911,7 +4926,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="50">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4919,10 +4934,10 @@
       <c r="C36" s="118" t="s">
         <v>127</v>
       </c>
-      <c r="D36" s="223" t="s">
+      <c r="D36" s="142" t="s">
         <v>120</v>
       </c>
-      <c r="E36" s="224"/>
+      <c r="E36" s="143"/>
       <c r="F36" s="33">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G36:$I36,-1)), "")</f>
         <v>3</v>
@@ -4944,15 +4959,15 @@
         <f>IFERROR(AVERAGE(F34:F38),"-")</f>
         <v>1.4</v>
       </c>
-      <c r="L36" s="164" t="str">
+      <c r="L36" s="206" t="str">
         <f>IF($F$36=1,"Please state the secure research environment being used, and explain the data security arrangments in place",IF($F$36=2,"Please state the research environment being used, and what precautions are being taken to ensure data security",IF($F$36=3,"This selection has passed a tolerance. Please state the research environment being used, and what arrangements are still to be considered","Please select an option in cell D36")))</f>
         <v>This selection has passed a tolerance. Please state the research environment being used, and what arrangements are still to be considered</v>
       </c>
-      <c r="M36" s="165"/>
-      <c r="N36" s="168" t="s">
-        <v>166</v>
-      </c>
-      <c r="O36" s="169"/>
+      <c r="M36" s="207"/>
+      <c r="N36" s="214" t="s">
+        <v>160</v>
+      </c>
+      <c r="O36" s="215"/>
       <c r="P36" s="16">
         <f>IF(SUM(I36)&gt;0, 1, 0)</f>
         <v>1</v>
@@ -4964,7 +4979,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="50">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4972,10 +4987,10 @@
       <c r="C37" s="121" t="s">
         <v>130</v>
       </c>
-      <c r="D37" s="223" t="s">
+      <c r="D37" s="142" t="s">
         <v>128</v>
       </c>
-      <c r="E37" s="224"/>
+      <c r="E37" s="143"/>
       <c r="F37" s="33">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G37:$I37,-1)), "")</f>
         <v>1</v>
@@ -4997,15 +5012,15 @@
         <f t="shared" ref="K37:K38" si="2">K36</f>
         <v>1.4</v>
       </c>
-      <c r="L37" s="164" t="str">
+      <c r="L37" s="206" t="str">
         <f>IF($F$37=1,"Please explain the measures in place to gain fully informed consent for this project",IF($F$37=2,"Please provide a justification as to why ethcial consent is not being sought for this particular project?",IF($F$37=3,"This selection has passed a tolerance. Please explain why consent is not being sought","Please select an option in cell D37")))</f>
         <v>Please explain the measures in place to gain fully informed consent for this project</v>
       </c>
-      <c r="M37" s="165"/>
-      <c r="N37" s="154" t="s">
-        <v>167</v>
-      </c>
-      <c r="O37" s="155"/>
+      <c r="M37" s="207"/>
+      <c r="N37" s="229" t="s">
+        <v>161</v>
+      </c>
+      <c r="O37" s="230"/>
       <c r="P37" s="16">
         <f>IF(SUM(I37)&gt;0, 1, 0)</f>
         <v>0</v>
@@ -5017,7 +5032,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="2:16 16381:16383" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="2:16 16381:16383" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="51">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -5025,10 +5040,10 @@
       <c r="C38" s="119" t="s">
         <v>133</v>
       </c>
-      <c r="D38" s="227" t="s">
+      <c r="D38" s="146" t="s">
         <v>138</v>
       </c>
-      <c r="E38" s="228"/>
+      <c r="E38" s="147"/>
       <c r="F38" s="34">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G38:$I38,-1)), "")</f>
         <v>1</v>
@@ -5053,15 +5068,15 @@
         <f t="shared" si="2"/>
         <v>1.4</v>
       </c>
-      <c r="L38" s="164" t="str">
+      <c r="L38" s="206" t="str">
         <f>IF($F$38=1,"Please outline the permissions that are in place",IF($F$38=2,"This selection has passed a tolerance. Please seek clarity on this issue",IF($F$38=3,"This selection has passed a tolerance. Please explain how you are going to ensure any outstanding data owner permissions are secured",IF($J$38=1,"In instances where permission is not needed, please provide a solid justification, along with evidence, to explain why permission is not required","Please select an option in cell D38"))))</f>
         <v>Please outline the permissions that are in place</v>
       </c>
-      <c r="M38" s="165"/>
-      <c r="N38" s="158" t="s">
-        <v>168</v>
-      </c>
-      <c r="O38" s="159"/>
+      <c r="M38" s="207"/>
+      <c r="N38" s="212" t="s">
+        <v>162</v>
+      </c>
+      <c r="O38" s="213"/>
       <c r="P38" s="16">
         <f>IF(SUM(H38:I38)&gt;0, 1, 0)</f>
         <v>0</v>
@@ -5073,15 +5088,15 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="2:16 16381:16383" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="2:16 16381:16383" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="20"/>
       <c r="C39" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="D39" s="174" t="s">
+      <c r="D39" s="161" t="s">
         <v>99</v>
       </c>
-      <c r="E39" s="175"/>
+      <c r="E39" s="160"/>
       <c r="F39" s="35" t="s">
         <v>100</v>
       </c>
@@ -5101,30 +5116,30 @@
         <f t="shared" ref="K39:K41" si="3">K40</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L39" s="150" t="s">
+      <c r="L39" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="M39" s="151"/>
-      <c r="N39" s="150" t="s">
+      <c r="M39" s="153"/>
+      <c r="N39" s="152" t="s">
         <v>103</v>
       </c>
-      <c r="O39" s="151"/>
+      <c r="O39" s="153"/>
       <c r="P39" s="16"/>
       <c r="XFA39" s="86" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="40" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="49">
         <v>10</v>
       </c>
       <c r="C40" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="229" t="s">
+      <c r="D40" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="230"/>
+      <c r="E40" s="149"/>
       <c r="F40" s="32">
         <f t="shared" ref="F40:F45" si="4">IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G40:$I40,-1)), "")</f>
         <v>1</v>
@@ -5146,15 +5161,15 @@
         <f t="shared" si="3"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L40" s="164" t="str">
+      <c r="L40" s="206" t="str">
         <f>IF($F$40=1,"Please explain why methods and data used will confidently lead to valid conclusions",IF($F$40=2,"Please explain why you have limited confidence/are unsure whether methods and data used will lead to valid conclusions, and provide mitigations against this uncertainty",IF($F$40=3,"This selection has passed a tolerance. Please explain why methods and data used may lead to invalid conclusions, justify the use of these methods or data, and provide any mitigations","Please select an option in cell D40")))</f>
         <v>Please explain why methods and data used will confidently lead to valid conclusions</v>
       </c>
-      <c r="M40" s="165"/>
-      <c r="N40" s="152" t="s">
-        <v>169</v>
-      </c>
-      <c r="O40" s="153"/>
+      <c r="M40" s="207"/>
+      <c r="N40" s="210" t="s">
+        <v>163</v>
+      </c>
+      <c r="O40" s="211"/>
       <c r="P40" s="16">
         <f>IF(SUM(I40:I40)&gt;0, 1, 0)</f>
         <v>0</v>
@@ -5163,7 +5178,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="50">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -5171,10 +5186,10 @@
       <c r="C41" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="170" t="s">
+      <c r="D41" s="150" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="171"/>
+      <c r="E41" s="151"/>
       <c r="F41" s="33">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -5196,15 +5211,15 @@
         <f t="shared" si="3"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L41" s="164" t="str">
+      <c r="L41" s="206" t="str">
         <f>IF($F$41=1,"Please explain the established research standards of the research organisation",IF($F$41=2,"Please explain why you have limited confidence/are unsure whether the organisation has established procedures",IF($F$41=3,"This selection has passed a tolerance. Please provide mitigations for this risk, and explain why research is to be done without clear and compliant procedures","Please select an option in cell D41")))</f>
         <v>Please explain the established research standards of the research organisation</v>
       </c>
-      <c r="M41" s="165"/>
-      <c r="N41" s="158" t="s">
-        <v>168</v>
-      </c>
-      <c r="O41" s="159"/>
+      <c r="M41" s="207"/>
+      <c r="N41" s="212" t="s">
+        <v>162</v>
+      </c>
+      <c r="O41" s="213"/>
       <c r="P41" s="16">
         <f>IF(SUM(I41)&gt;0, 1, 0)</f>
         <v>0</v>
@@ -5213,7 +5228,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="50">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -5221,10 +5236,10 @@
       <c r="C42" s="118" t="s">
         <v>35</v>
       </c>
-      <c r="D42" s="170" t="s">
+      <c r="D42" s="150" t="s">
         <v>38</v>
       </c>
-      <c r="E42" s="171"/>
+      <c r="E42" s="151"/>
       <c r="F42" s="33">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -5246,15 +5261,15 @@
         <f>IFERROR(AVERAGE(F40:F45),"-")</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L42" s="164" t="str">
+      <c r="L42" s="206" t="str">
         <f>IF($F$42=1,"Please explain the training that researchers have received to do this research",IF($F$42=2,"Please explain why researchers are to be used with limited training, and provide a mitigation agasint this limitation",IF($F$42=3,"This selection has passed a tolerance. Please explain the training that has been recieved, and why there is limited assurance that it relates to this research","Please select an option in cell D42")))</f>
         <v>Please explain the training that researchers have received to do this research</v>
       </c>
-      <c r="M42" s="165"/>
-      <c r="N42" s="158" t="s">
-        <v>171</v>
-      </c>
-      <c r="O42" s="159"/>
+      <c r="M42" s="207"/>
+      <c r="N42" s="212" t="s">
+        <v>165</v>
+      </c>
+      <c r="O42" s="213"/>
       <c r="P42" s="16">
         <f>IF(SUM(I42:I42)&gt;0, 1, 0)</f>
         <v>0</v>
@@ -5263,7 +5278,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="2:16 16381:16383" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="2:16 16381:16383" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="50">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -5271,10 +5286,10 @@
       <c r="C43" s="118" t="s">
         <v>141</v>
       </c>
-      <c r="D43" s="170" t="s">
+      <c r="D43" s="150" t="s">
         <v>52</v>
       </c>
-      <c r="E43" s="171"/>
+      <c r="E43" s="151"/>
       <c r="F43" s="33">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -5299,15 +5314,15 @@
         <f t="shared" ref="K43:K45" si="5">K42</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L43" s="164" t="str">
+      <c r="L43" s="206" t="str">
         <f>IF($F$43=1,"Please explain the planned human oversight processes for this project",IF($F$43=2,"Please explain the level of human oversight, and explain why it is limited",IF($F$43=3,"This selection has passed a tolerance. Please explain why there is minimal human oversight and provide a mitigation for this",IF($J$43=1,"Please justify the omission of this item","Please select an option in cell D43"))))</f>
         <v>Please explain the planned human oversight processes for this project</v>
       </c>
-      <c r="M43" s="165"/>
-      <c r="N43" s="154" t="s">
-        <v>170</v>
-      </c>
-      <c r="O43" s="155"/>
+      <c r="M43" s="207"/>
+      <c r="N43" s="229" t="s">
+        <v>164</v>
+      </c>
+      <c r="O43" s="230"/>
       <c r="P43" s="16">
         <f>IF(SUM(I43:I43)&gt;0, 1, 0)</f>
         <v>0</v>
@@ -5316,7 +5331,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="50">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -5324,10 +5339,10 @@
       <c r="C44" s="121" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="170" t="s">
+      <c r="D44" s="150" t="s">
         <v>77</v>
       </c>
-      <c r="E44" s="171"/>
+      <c r="E44" s="151"/>
       <c r="F44" s="33">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -5352,22 +5367,22 @@
         <f t="shared" si="5"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L44" s="164" t="str">
+      <c r="L44" s="206" t="str">
         <f>IF($F$44=1,"Please briefly outline the standard methods and technologies used",IF($F$44=2,"Please justify the use of this method, and provide mitigations against the risk of automation and/or using novel methods",IF($F$44=3,"This selection has passed a tolerance. Please justify the use of this method/tool, and provide mitigations",IF($J$44=1,"Please justify the omission of this item","Please select an option in cell D44"))))</f>
         <v>Please briefly outline the standard methods and technologies used</v>
       </c>
-      <c r="M44" s="165"/>
-      <c r="N44" s="154" t="s">
-        <v>172</v>
-      </c>
-      <c r="O44" s="155"/>
+      <c r="M44" s="207"/>
+      <c r="N44" s="229" t="s">
+        <v>166</v>
+      </c>
+      <c r="O44" s="230"/>
       <c r="P44" s="114">
         <f>IF(SUM(I44)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="XFC44" s="62"/>
     </row>
-    <row r="45" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="51">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5375,10 +5390,10 @@
       <c r="C45" s="122" t="s">
         <v>95</v>
       </c>
-      <c r="D45" s="172" t="s">
+      <c r="D45" s="157" t="s">
         <v>109</v>
       </c>
-      <c r="E45" s="173"/>
+      <c r="E45" s="158"/>
       <c r="F45" s="34">
         <f t="shared" si="4"/>
         <v>2</v>
@@ -5400,29 +5415,29 @@
         <f t="shared" si="5"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L45" s="164" t="str">
+      <c r="L45" s="206" t="str">
         <f>IF($F$45=1,"Please justify your confidence that the public good will be realised",IF($F$45=2,"Please explain why there is limited confidence/it is unsure that the public good will be realised, and justify why research should occur nonetheless",IF($F$45=3,"This selection has passed a tolerance. Please explain why the methods and data are still being pursued if there is little/no chance of the public good being realised","Please select an option in cell D45")))</f>
         <v>Please explain why there is limited confidence/it is unsure that the public good will be realised, and justify why research should occur nonetheless</v>
       </c>
-      <c r="M45" s="165"/>
-      <c r="N45" s="160" t="s">
-        <v>173</v>
-      </c>
-      <c r="O45" s="161"/>
+      <c r="M45" s="207"/>
+      <c r="N45" s="233" t="s">
+        <v>167</v>
+      </c>
+      <c r="O45" s="234"/>
       <c r="P45" s="16">
         <f>IF(SUM(I45:I45)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:16 16381:16383" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="2:16 16381:16383" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="20"/>
       <c r="C46" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="D46" s="174" t="s">
+      <c r="D46" s="161" t="s">
         <v>99</v>
       </c>
-      <c r="E46" s="175"/>
+      <c r="E46" s="160"/>
       <c r="F46" s="35" t="s">
         <v>100</v>
       </c>
@@ -5442,27 +5457,27 @@
         <f>K47</f>
         <v>1</v>
       </c>
-      <c r="L46" s="150" t="s">
+      <c r="L46" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="M46" s="151"/>
-      <c r="N46" s="150" t="s">
+      <c r="M46" s="153"/>
+      <c r="N46" s="152" t="s">
         <v>103</v>
       </c>
-      <c r="O46" s="151"/>
+      <c r="O46" s="153"/>
       <c r="P46" s="115"/>
     </row>
-    <row r="47" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:16 16381:16383" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="49">
         <v>16</v>
       </c>
       <c r="C47" s="123" t="s">
         <v>144</v>
       </c>
-      <c r="D47" s="225" t="s">
+      <c r="D47" s="144" t="s">
         <v>118</v>
       </c>
-      <c r="E47" s="226"/>
+      <c r="E47" s="145"/>
       <c r="F47" s="32">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G47:$I47,-1)), "")</f>
         <v>1</v>
@@ -5484,21 +5499,21 @@
         <f>IFERROR(AVERAGE(F47:F48),"-")</f>
         <v>1</v>
       </c>
-      <c r="L47" s="187" t="str">
+      <c r="L47" s="204" t="str">
         <f>IF($F$47=1,"Which legal gateways are required to facilitate this research? You may wish to consult the guidance document.",IF($F$47=2,"This selection has passed a tolerance. Please consult with available legal services support to confirm",IF($F$47=3,"This selection has passed a tolerance. Legality must be confirmed, please consult with available legal services support before proceeding","Please select an option in cell D47")))</f>
         <v>Which legal gateways are required to facilitate this research? You may wish to consult the guidance document.</v>
       </c>
-      <c r="M47" s="188"/>
-      <c r="N47" s="152" t="s">
-        <v>168</v>
-      </c>
-      <c r="O47" s="153"/>
+      <c r="M47" s="205"/>
+      <c r="N47" s="210" t="s">
+        <v>162</v>
+      </c>
+      <c r="O47" s="211"/>
       <c r="P47" s="114">
         <f>IF(SUM(H47:I47)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:16 16381:16383" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="2:16 16381:16383" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B48" s="51">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -5506,10 +5521,10 @@
       <c r="C48" s="124" t="s">
         <v>145</v>
       </c>
-      <c r="D48" s="227" t="s">
+      <c r="D48" s="146" t="s">
         <v>129</v>
       </c>
-      <c r="E48" s="228"/>
+      <c r="E48" s="147"/>
       <c r="F48" s="34">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G48:$I48,-1)), "")</f>
         <v>1</v>
@@ -5531,29 +5546,29 @@
         <f>K47</f>
         <v>1</v>
       </c>
-      <c r="L48" s="185" t="str">
+      <c r="L48" s="202" t="str">
         <f>IF($F$48=1,"Which are the legal frameworks pertinent to this project? You may wish to consult the guidance document.",IF($F$48=2,"This selection has passed a tolerance. Please consult with available legal services support to conflrm",IF($F$48=3,"This selection has passed a tolerance. Legality must be confirmed, please consult with available legal services support before proceeding","Please select an option in cell D48")))</f>
         <v>Which are the legal frameworks pertinent to this project? You may wish to consult the guidance document.</v>
       </c>
-      <c r="M48" s="186"/>
-      <c r="N48" s="158" t="s">
-        <v>168</v>
-      </c>
-      <c r="O48" s="159"/>
+      <c r="M48" s="203"/>
+      <c r="N48" s="212" t="s">
+        <v>162</v>
+      </c>
+      <c r="O48" s="213"/>
       <c r="P48" s="16">
         <f>IF(SUM(H48:I48)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B49" s="20"/>
       <c r="C49" s="54" t="s">
         <v>146</v>
       </c>
-      <c r="D49" s="174" t="s">
+      <c r="D49" s="161" t="s">
         <v>99</v>
       </c>
-      <c r="E49" s="175"/>
+      <c r="E49" s="160"/>
       <c r="F49" s="35" t="s">
         <v>100</v>
       </c>
@@ -5573,27 +5588,27 @@
         <f>K50</f>
         <v>3</v>
       </c>
-      <c r="L49" s="150" t="s">
+      <c r="L49" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="M49" s="151"/>
-      <c r="N49" s="150" t="s">
+      <c r="M49" s="153"/>
+      <c r="N49" s="152" t="s">
         <v>103</v>
       </c>
-      <c r="O49" s="151"/>
+      <c r="O49" s="153"/>
       <c r="P49" s="16"/>
     </row>
-    <row r="50" spans="2:16" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="2:16" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B50" s="52">
         <v>18</v>
       </c>
       <c r="C50" s="120" t="s">
         <v>147</v>
       </c>
-      <c r="D50" s="229" t="s">
+      <c r="D50" s="148" t="s">
         <v>16</v>
       </c>
-      <c r="E50" s="230"/>
+      <c r="E50" s="149"/>
       <c r="F50" s="32">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G50:$I50,-1)), "")</f>
         <v>3</v>
@@ -5615,21 +5630,21 @@
         <f>IFERROR(AVERAGE(F50:F51), "-")</f>
         <v>3</v>
       </c>
-      <c r="L50" s="187" t="str">
+      <c r="L50" s="204" t="str">
         <f>IF($F$50=1,"Please explain the positive public views, and evidence how this is known",IF($F$50=2,"Please explain the limited public support, evidence how this is known, and provide a mitigation",IF($F$50=3,"This selection has passed a tolerance. Either explain and justify why the views are unknown or explain the public's negative views, and evidence how this is known","Please select an option in cell D50")))</f>
         <v>This selection has passed a tolerance. Either explain and justify why the views are unknown or explain the public's negative views, and evidence how this is known</v>
       </c>
-      <c r="M50" s="188"/>
-      <c r="N50" s="152" t="s">
-        <v>174</v>
-      </c>
-      <c r="O50" s="153"/>
+      <c r="M50" s="205"/>
+      <c r="N50" s="210" t="s">
+        <v>168</v>
+      </c>
+      <c r="O50" s="211"/>
       <c r="P50" s="16">
         <f>IF(SUM(I50)&gt;0, 1, 0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:16" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="2:16" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="51">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -5637,10 +5652,10 @@
       <c r="C51" s="119" t="s">
         <v>21</v>
       </c>
-      <c r="D51" s="172" t="s">
+      <c r="D51" s="157" t="s">
         <v>33</v>
       </c>
-      <c r="E51" s="173"/>
+      <c r="E51" s="158"/>
       <c r="F51" s="34">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G51:$I51,-1)), "")</f>
         <v>3</v>
@@ -5665,29 +5680,29 @@
         <f>K50</f>
         <v>3</v>
       </c>
-      <c r="L51" s="164" t="str">
+      <c r="L51" s="206" t="str">
         <f>IF($F$51=1,"Please outline the planned regular public engagement",IF($F$51=2,"Please outline the engagement planned, and justify why it is not regular throughout the project",IF($F$51=3,"This selection has passed a tolerance. Please explain and justify why no public engagement is planned or required",IF($J$51=1,"Please explain why public engagment is not needed for this project","Please select an option in cell D51"))))</f>
         <v>This selection has passed a tolerance. Please explain and justify why no public engagement is planned or required</v>
       </c>
-      <c r="M51" s="165"/>
-      <c r="N51" s="152" t="s">
+      <c r="M51" s="207"/>
+      <c r="N51" s="210" t="s">
         <v>175</v>
       </c>
-      <c r="O51" s="153"/>
+      <c r="O51" s="211"/>
       <c r="P51" s="16">
         <f>IF(SUM(I51)&gt;0, 1, 0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="2:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="21"/>
       <c r="C52" s="54" t="s">
         <v>148</v>
       </c>
-      <c r="D52" s="174" t="s">
+      <c r="D52" s="161" t="s">
         <v>99</v>
       </c>
-      <c r="E52" s="175"/>
+      <c r="E52" s="160"/>
       <c r="F52" s="35" t="s">
         <v>100</v>
       </c>
@@ -5707,27 +5722,27 @@
         <f>K53</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="L52" s="150" t="s">
+      <c r="L52" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="M52" s="151"/>
-      <c r="N52" s="150" t="s">
+      <c r="M52" s="153"/>
+      <c r="N52" s="152" t="s">
         <v>103</v>
       </c>
-      <c r="O52" s="151"/>
+      <c r="O52" s="153"/>
       <c r="P52" s="16"/>
     </row>
-    <row r="53" spans="2:16" ht="120" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:16" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="49">
         <v>20</v>
       </c>
       <c r="C53" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="D53" s="225" t="s">
+      <c r="D53" s="144" t="s">
         <v>47</v>
       </c>
-      <c r="E53" s="226"/>
+      <c r="E53" s="145"/>
       <c r="F53" s="32">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G53:$I53,-1)), "")</f>
         <v>2</v>
@@ -5749,21 +5764,21 @@
         <f>IFERROR(AVERAGE(F53:F55),"-")</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="L53" s="187" t="str">
+      <c r="L53" s="204" t="str">
         <f>IF($F$53=1,"Please explain how research outcomes will be made openly available to the public",IF($F$53=2,"This selection has passed a tolerance. Please explain why the potential for public access to outcomes is unknown",IF($F$53=3,"This selection has passed a tolerance. Please explain why outcomes will not be openly available to the public","Please select an option in cell D53")))</f>
         <v>This selection has passed a tolerance. Please explain why the potential for public access to outcomes is unknown</v>
       </c>
-      <c r="M53" s="188"/>
-      <c r="N53" s="152" t="s">
-        <v>178</v>
-      </c>
-      <c r="O53" s="153"/>
+      <c r="M53" s="205"/>
+      <c r="N53" s="210" t="s">
+        <v>176</v>
+      </c>
+      <c r="O53" s="211"/>
       <c r="P53" s="16">
         <f>IF(SUM(H53:I53)&gt;0, 1, 0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:16" ht="120" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:16" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="50">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -5771,10 +5786,10 @@
       <c r="C54" s="125" t="s">
         <v>149</v>
       </c>
-      <c r="D54" s="170" t="s">
+      <c r="D54" s="150" t="s">
         <v>66</v>
       </c>
-      <c r="E54" s="171"/>
+      <c r="E54" s="151"/>
       <c r="F54" s="33">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G54:$I54,-1)), "")</f>
         <v>2</v>
@@ -5799,21 +5814,21 @@
         <f t="shared" ref="K54:K55" si="6">K53</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="L54" s="164" t="str">
+      <c r="L54" s="206" t="str">
         <f>IF($F$54=1,"Please explain how methods and tools will be openly available to the public",IF($F$54=2,"Please explain why the sharing of methods and/or tools is unknown?",IF($F$54=3,"This selection has passed a tolerance. Please explain why methods and/or will not be openly available to the public",IF($J$54=1,"Please explain the omission of this item","Please select an option in cell D54"))))</f>
         <v>Please explain why the sharing of methods and/or tools is unknown?</v>
       </c>
-      <c r="M54" s="165"/>
-      <c r="N54" s="154" t="s">
-        <v>177</v>
-      </c>
-      <c r="O54" s="155"/>
+      <c r="M54" s="207"/>
+      <c r="N54" s="229" t="s">
+        <v>170</v>
+      </c>
+      <c r="O54" s="230"/>
       <c r="P54" s="16">
         <f>IF(SUM(I54)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:16" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="2:16" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="53">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -5821,10 +5836,10 @@
       <c r="C55" s="124" t="s">
         <v>78</v>
       </c>
-      <c r="D55" s="172" t="s">
+      <c r="D55" s="157" t="s">
         <v>81</v>
       </c>
-      <c r="E55" s="173"/>
+      <c r="E55" s="158"/>
       <c r="F55" s="36">
         <f>IFERROR(INDEX($G$28:$I$28,0,MATCH(0,$G55:$I55,-1)), "")</f>
         <v>1</v>
@@ -5849,73 +5864,161 @@
         <f t="shared" si="6"/>
         <v>1.6666666666666667</v>
       </c>
-      <c r="L55" s="183" t="str">
+      <c r="L55" s="200" t="str">
         <f>IF($F$55=1,"Please state the data retention policy for this project, and explain how the data will be available for re-use",IF($F$55=2,"Please explain why the re-use of data is unknown, and/or why are data retention polcies unclear?",IF($F$55=3,"This selection has passed a tolerance. Please explain why data will not be availabe for re-use, or why data retention policies are not in place",IF($J$55=1,"Please explain why the dataset(s) cannot be re-used","Please select an option in cell D55"))))</f>
         <v>Please state the data retention policy for this project, and explain how the data will be available for re-use</v>
       </c>
-      <c r="M55" s="184"/>
-      <c r="N55" s="156" t="s">
-        <v>176</v>
-      </c>
-      <c r="O55" s="157"/>
+      <c r="M55" s="201"/>
+      <c r="N55" s="231" t="s">
+        <v>169</v>
+      </c>
+      <c r="O55" s="232"/>
       <c r="P55" s="16">
         <f>IF(SUM(I55)&gt;0, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:16" ht="54" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:16" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L56" s="59"/>
       <c r="M56" s="59"/>
       <c r="P56" s="22"/>
     </row>
-    <row r="57" spans="2:16" ht="47.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="N57" s="137" t="s">
+    <row r="57" spans="2:16" ht="47.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N57" s="216" t="s">
         <v>150</v>
       </c>
-      <c r="O57" s="137"/>
-    </row>
-    <row r="66" spans="16:16" hidden="1" x14ac:dyDescent="0.5">
-      <c r="P66" s="220"/>
-    </row>
-    <row r="67" spans="16:16" hidden="1" x14ac:dyDescent="0.5">
-      <c r="P67" s="220"/>
-    </row>
-    <row r="68" spans="16:16" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="P68" s="220"/>
-    </row>
-    <row r="69" spans="16:16" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="P69" s="220"/>
-    </row>
-    <row r="70" spans="16:16" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="P70" s="220"/>
-    </row>
-    <row r="71" spans="16:16" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="P71" s="220"/>
-    </row>
-    <row r="72" spans="16:16" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="P72" s="220"/>
-    </row>
-    <row r="73" spans="16:16" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="P73" s="220"/>
-    </row>
-    <row r="74" spans="16:16" hidden="1" x14ac:dyDescent="0.5">
-      <c r="P74" s="220"/>
-    </row>
-    <row r="75" spans="16:16" hidden="1" x14ac:dyDescent="0.5">
-      <c r="P75" s="220"/>
-    </row>
-    <row r="76" spans="16:16" hidden="1" x14ac:dyDescent="0.5">
-      <c r="P76" s="220"/>
-    </row>
-    <row r="77" spans="16:16" hidden="1" x14ac:dyDescent="0.5">
-      <c r="P77" s="220"/>
-    </row>
-    <row r="1048576" spans="15:15" hidden="1" x14ac:dyDescent="0.5">
+      <c r="O57" s="216"/>
+    </row>
+    <row r="66" spans="16:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="P66" s="139"/>
+    </row>
+    <row r="67" spans="16:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="P67" s="139"/>
+    </row>
+    <row r="68" spans="16:16" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P68" s="139"/>
+    </row>
+    <row r="69" spans="16:16" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P69" s="139"/>
+    </row>
+    <row r="70" spans="16:16" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P70" s="139"/>
+    </row>
+    <row r="71" spans="16:16" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P71" s="139"/>
+    </row>
+    <row r="72" spans="16:16" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P72" s="139"/>
+    </row>
+    <row r="73" spans="16:16" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P73" s="139"/>
+    </row>
+    <row r="74" spans="16:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="P74" s="139"/>
+    </row>
+    <row r="75" spans="16:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="P75" s="139"/>
+    </row>
+    <row r="76" spans="16:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="P76" s="139"/>
+    </row>
+    <row r="77" spans="16:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="P77" s="139"/>
+    </row>
+    <row r="1048576" spans="15:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="O1048576" s="59"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BQmOtmUROdBToi7l77hhhud6Bo0c/G4ZFtWzh7lYkH91HMJj1Z280byvkwYlS2ZyOGJEpIQYeLG0ZD1SnN9gwA==" saltValue="N19zbME1rV6I1G6Ha2uGcg==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatRows="0" selectLockedCells="1"/>
   <mergeCells count="112">
+    <mergeCell ref="N57:O57"/>
+    <mergeCell ref="M21:N24"/>
+    <mergeCell ref="L19:N20"/>
+    <mergeCell ref="N52:O52"/>
+    <mergeCell ref="N53:O53"/>
+    <mergeCell ref="N54:O54"/>
+    <mergeCell ref="N55:O55"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="N50:O50"/>
+    <mergeCell ref="N51:O51"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="L55:M55"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="L50:M50"/>
+    <mergeCell ref="L51:M51"/>
+    <mergeCell ref="L52:M52"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="L54:M54"/>
+    <mergeCell ref="L53:M53"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="L21:L24"/>
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="C7:L7"/>
+    <mergeCell ref="C10:L10"/>
+    <mergeCell ref="C13:L13"/>
+    <mergeCell ref="C16:L16"/>
+    <mergeCell ref="C6:L6"/>
+    <mergeCell ref="C9:L9"/>
+    <mergeCell ref="C12:L12"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C8:L8"/>
     <mergeCell ref="P66:P77"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D37:E37"/>
@@ -5940,94 +6043,6 @@
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="D43:E43"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="L21:L24"/>
-    <mergeCell ref="C4:L4"/>
-    <mergeCell ref="C7:L7"/>
-    <mergeCell ref="C10:L10"/>
-    <mergeCell ref="C13:L13"/>
-    <mergeCell ref="C16:L16"/>
-    <mergeCell ref="C6:L6"/>
-    <mergeCell ref="C9:L9"/>
-    <mergeCell ref="C12:L12"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="L55:M55"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="L50:M50"/>
-    <mergeCell ref="L51:M51"/>
-    <mergeCell ref="L52:M52"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="L54:M54"/>
-    <mergeCell ref="L53:M53"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="N57:O57"/>
-    <mergeCell ref="M21:N24"/>
-    <mergeCell ref="L19:N20"/>
-    <mergeCell ref="N52:O52"/>
-    <mergeCell ref="N53:O53"/>
-    <mergeCell ref="N54:O54"/>
-    <mergeCell ref="N55:O55"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="N48:O48"/>
-    <mergeCell ref="N49:O49"/>
-    <mergeCell ref="N50:O50"/>
-    <mergeCell ref="N51:O51"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="N33:O33"/>
   </mergeCells>
   <conditionalFormatting sqref="B19:D19 H19">
     <cfRule type="containsText" dxfId="45" priority="38" operator="containsText" text="Have you considered these questions?">
@@ -6623,6 +6638,11 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Retention xmlns="6dab36e7-c487-4780-8e35-3b48fa83d7a8">0</Retention>
@@ -6632,11 +6652,6 @@
     <RetentionType xmlns="6dab36e7-c487-4780-8e35-3b48fa83d7a8">Notify</RetentionType>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6659,6 +6674,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BA0B1F6-4CF4-4794-A965-695655EABB38}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{682AC2EE-0B14-436F-A00B-D74F0C6291E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -6666,12 +6689,4 @@
     <ds:schemaRef ds:uri="6dab36e7-c487-4780-8e35-3b48fa83d7a8"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BA0B1F6-4CF4-4794-A965-695655EABB38}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>